<commit_message>
RGB LED Wrapper/Graphics POC
</commit_message>
<xml_diff>
--- a/documentation/Pendulum General Notes.xlsx
+++ b/documentation/Pendulum General Notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ross\Documents\GitHub\Furuta-Pendulum\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Github_Repos\Furuta-Pendulum\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C5C8A6-A6A7-4862-89E1-560AB0F6E9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A279326-1E3B-4472-B59B-4C7A49709E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NXP15XH103F03RC " sheetId="5" r:id="rId1"/>
@@ -513,7 +513,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -553,10 +553,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,16 +1062,16 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>151</v>
       </c>
@@ -1079,17 +1079,17 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>147</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>146</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>145</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>144</v>
       </c>
@@ -1122,12 +1122,12 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
       <c r="H21">
         <v>274.14999999999998</v>
       </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>143</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>3455</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>54.039423557411865</v>
       </c>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>3455</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>97.82536621618496</v>
       </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>3455</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>167.72873235490044</v>
       </c>
     </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>3455</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>273.09089816363326</v>
       </c>
     </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>3455</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>3455</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>622.93869172748441</v>
       </c>
     </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>3455</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>3455</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>1168.1899374657055</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>3455</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>1491.7416415985278</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>3455</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>1825.7304907981015</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>3455</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>2151.396943141714</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>3455</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>2453.7008277400541</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>3455</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>2723.2172426961902</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>3455</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>2956.0577198229148</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>3455</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>3152.5786257994127</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>3455</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>3315.7626168202719</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>3455</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>3449.8361873826639</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E42">
         <v>3455</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>3559.3192522629574</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>3455</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>3648.4778466001449</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>3455</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>3721.0689591442965</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E45">
         <v>3455</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>3780.2656325848657</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E46">
         <v>3455</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>3828.6787150076775</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E47">
         <v>3455</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>3868.4219508381043</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>3455</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>3901.1901499119167</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E49">
         <v>3455</v>
       </c>
@@ -1703,127 +1703,127 @@
         <v>3928.3351114386833</v>
       </c>
     </row>
-    <row r="55" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F55">
         <v>-40</v>
       </c>
     </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F56">
         <v>-30</v>
       </c>
     </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F57">
         <v>-20</v>
       </c>
     </row>
-    <row r="58" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F58">
         <v>-10</v>
       </c>
     </row>
-    <row r="59" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F60">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F61">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F62">
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F63">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F64">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F66">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68">
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F69">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F70">
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F71">
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F72">
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F73">
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F74">
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F75">
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F76">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F77">
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F78">
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F79">
         <v>200</v>
       </c>
@@ -1839,25 +1839,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0F148E-F223-466A-A7C9-AAB69A928868}">
   <dimension ref="C11:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="77" workbookViewId="0">
-      <selection activeCell="L143" sqref="L143"/>
+    <sheetView topLeftCell="B2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <f>1/(((D14/100*3)+1)^3)</f>
         <v>1</v>
       </c>
@@ -1868,16 +1868,16 @@
         <v>154</v>
       </c>
       <c r="I14">
-        <f>255*E14</f>
+        <f t="shared" ref="I14:I45" si="0">255*E14</f>
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="7">
-        <f t="shared" ref="E15:E78" si="0">1/(((D15/100*3)+1)^3)</f>
+      <c r="E15" s="6">
+        <f t="shared" ref="E15:E78" si="1">1/(((D15/100*3)+1)^3)</f>
         <v>0.91514165935315961</v>
       </c>
       <c r="F15" t="s">
@@ -1887,586 +1887,586 @@
         <v>154</v>
       </c>
       <c r="I15">
-        <f>255*E15</f>
+        <f t="shared" si="0"/>
         <v>233.36112313505569</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>2</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
+        <f t="shared" si="1"/>
+        <v>0.8396192830323016</v>
+      </c>
+      <c r="F16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="0"/>
-        <v>0.8396192830323016</v>
-      </c>
-      <c r="F16" t="s">
-        <v>153</v>
-      </c>
-      <c r="G16" t="s">
-        <v>154</v>
-      </c>
-      <c r="I16">
-        <f>255*E16</f>
         <v>214.1029171732369</v>
       </c>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>3</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
+        <f t="shared" si="1"/>
+        <v>0.77218348006106419</v>
+      </c>
+      <c r="F17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" t="s">
+        <v>154</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="0"/>
-        <v>0.77218348006106419</v>
-      </c>
-      <c r="F17" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" t="s">
-        <v>154</v>
-      </c>
-      <c r="I17">
-        <f>255*E17</f>
         <v>196.90678741557136</v>
       </c>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>4</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
+        <f t="shared" si="1"/>
+        <v>0.71178024781341087</v>
+      </c>
+      <c r="F18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" t="s">
+        <v>154</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="0"/>
-        <v>0.71178024781341087</v>
-      </c>
-      <c r="F18" t="s">
-        <v>153</v>
-      </c>
-      <c r="G18" t="s">
-        <v>154</v>
-      </c>
-      <c r="I18">
-        <f>255*E18</f>
         <v>181.50396319241977</v>
       </c>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>5</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
+        <f t="shared" si="1"/>
+        <v>0.65751623243198831</v>
+      </c>
+      <c r="F19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G19" t="s">
+        <v>154</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="0"/>
-        <v>0.65751623243198831</v>
-      </c>
-      <c r="F19" t="s">
-        <v>153</v>
-      </c>
-      <c r="G19" t="s">
-        <v>154</v>
-      </c>
-      <c r="I19">
-        <f>255*E19</f>
         <v>167.66663927015702</v>
       </c>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>6</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
+        <f t="shared" si="1"/>
+        <v>0.6086308726792905</v>
+      </c>
+      <c r="F20" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" t="s">
+        <v>154</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="0"/>
-        <v>0.6086308726792905</v>
-      </c>
-      <c r="F20" t="s">
-        <v>153</v>
-      </c>
-      <c r="G20" t="s">
-        <v>154</v>
-      </c>
-      <c r="I20">
-        <f>255*E20</f>
         <v>155.20087253321907</v>
       </c>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>7</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
+        <f t="shared" si="1"/>
+        <v>0.56447393005377744</v>
+      </c>
+      <c r="F21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G21" t="s">
+        <v>154</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="0"/>
-        <v>0.56447393005377744</v>
-      </c>
-      <c r="F21" t="s">
-        <v>153</v>
-      </c>
-      <c r="G21" t="s">
-        <v>154</v>
-      </c>
-      <c r="I21">
-        <f>255*E21</f>
         <v>143.94085216371326</v>
       </c>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>8</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
+        <f>1/(((D22/100*3)+1)^3)</f>
+        <v>0.52448726125339862</v>
+      </c>
+      <c r="F22" t="s">
+        <v>153</v>
+      </c>
+      <c r="G22" t="s">
+        <v>154</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="0"/>
-        <v>0.52448726125339862</v>
-      </c>
-      <c r="F22" t="s">
-        <v>153</v>
-      </c>
-      <c r="G22" t="s">
-        <v>154</v>
-      </c>
-      <c r="I22">
-        <f>255*E22</f>
         <v>133.74425161961665</v>
       </c>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>9</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
+        <f t="shared" si="1"/>
+        <v>0.48818995275785831</v>
+      </c>
+      <c r="F23" t="s">
+        <v>153</v>
+      </c>
+      <c r="G23" t="s">
+        <v>154</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="0"/>
-        <v>0.48818995275785831</v>
-      </c>
-      <c r="F23" t="s">
-        <v>153</v>
-      </c>
-      <c r="G23" t="s">
-        <v>154</v>
-      </c>
-      <c r="I23">
-        <f>255*E23</f>
         <v>124.48843795325386</v>
       </c>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>10</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
+        <f t="shared" si="1"/>
+        <v>0.45516613563950831</v>
+      </c>
+      <c r="F24" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" t="s">
+        <v>154</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="0"/>
-        <v>0.45516613563950831</v>
-      </c>
-      <c r="F24" t="s">
-        <v>153</v>
-      </c>
-      <c r="G24" t="s">
-        <v>154</v>
-      </c>
-      <c r="I24">
-        <f>255*E24</f>
         <v>116.06736458807462</v>
       </c>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>11</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
+        <f t="shared" si="1"/>
+        <v>0.42505494897852919</v>
+      </c>
+      <c r="F25" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" t="s">
+        <v>154</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="0"/>
-        <v>0.42505494897852919</v>
-      </c>
-      <c r="F25" t="s">
-        <v>153</v>
-      </c>
-      <c r="G25" t="s">
-        <v>154</v>
-      </c>
-      <c r="I25">
-        <f>255*E25</f>
         <v>108.38901198952495</v>
       </c>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>12</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
+        <f t="shared" si="1"/>
+        <v>0.3975422348870345</v>
+      </c>
+      <c r="F26" t="s">
+        <v>153</v>
+      </c>
+      <c r="G26" t="s">
+        <v>154</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="0"/>
-        <v>0.3975422348870345</v>
-      </c>
-      <c r="F26" t="s">
-        <v>153</v>
-      </c>
-      <c r="G26" t="s">
-        <v>154</v>
-      </c>
-      <c r="I26">
-        <f>255*E26</f>
         <v>101.37326989619379</v>
       </c>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>13</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
+        <f t="shared" si="1"/>
+        <v>0.3723536361635808</v>
+      </c>
+      <c r="F27" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" t="s">
+        <v>154</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="0"/>
-        <v>0.3723536361635808</v>
-      </c>
-      <c r="F27" t="s">
-        <v>153</v>
-      </c>
-      <c r="G27" t="s">
-        <v>154</v>
-      </c>
-      <c r="I27">
-        <f>255*E27</f>
         <v>94.950177221713105</v>
       </c>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>14</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
+        <f t="shared" si="1"/>
+        <v>0.34924883560438214</v>
+      </c>
+      <c r="F28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" t="s">
+        <v>154</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="0"/>
-        <v>0.34924883560438214</v>
-      </c>
-      <c r="F28" t="s">
-        <v>153</v>
-      </c>
-      <c r="G28" t="s">
-        <v>154</v>
-      </c>
-      <c r="I28">
-        <f>255*E28</f>
         <v>89.058453079117442</v>
       </c>
     </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>15</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
+        <f t="shared" si="1"/>
+        <v>0.32801672885317151</v>
+      </c>
+      <c r="F29" t="s">
+        <v>153</v>
+      </c>
+      <c r="G29" t="s">
+        <v>154</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="0"/>
-        <v>0.32801672885317151</v>
-      </c>
-      <c r="F29" t="s">
-        <v>153</v>
-      </c>
-      <c r="G29" t="s">
-        <v>154</v>
-      </c>
-      <c r="I29">
-        <f>255*E29</f>
         <v>83.644265857558736</v>
       </c>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>16</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
+        <f t="shared" si="1"/>
+        <v>0.30847136398633845</v>
+      </c>
+      <c r="F30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" t="s">
+        <v>154</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="0"/>
-        <v>0.30847136398633845</v>
-      </c>
-      <c r="F30" t="s">
-        <v>153</v>
-      </c>
-      <c r="G30" t="s">
-        <v>154</v>
-      </c>
-      <c r="I30">
-        <f>255*E30</f>
         <v>78.660197816516302</v>
       </c>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>17</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
+        <f t="shared" si="1"/>
+        <v>0.29044851349903034</v>
+      </c>
+      <c r="F31" t="s">
+        <v>153</v>
+      </c>
+      <c r="G31" t="s">
+        <v>154</v>
+      </c>
+      <c r="I31">
         <f t="shared" si="0"/>
-        <v>0.29044851349903034</v>
-      </c>
-      <c r="F31" t="s">
-        <v>153</v>
-      </c>
-      <c r="G31" t="s">
-        <v>154</v>
-      </c>
-      <c r="I31">
-        <f>255*E31</f>
         <v>74.064370942252737</v>
       </c>
     </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>18</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
+        <f t="shared" si="1"/>
+        <v>0.27380277000786363</v>
+      </c>
+      <c r="F32" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32" t="s">
+        <v>154</v>
+      </c>
+      <c r="I32">
         <f t="shared" si="0"/>
-        <v>0.27380277000786363</v>
-      </c>
-      <c r="F32" t="s">
-        <v>153</v>
-      </c>
-      <c r="G32" t="s">
-        <v>154</v>
-      </c>
-      <c r="I32">
-        <f>255*E32</f>
         <v>69.819706352005227</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>19</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
+        <f t="shared" si="1"/>
+        <v>0.25840507734968382</v>
+      </c>
+      <c r="F33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" t="s">
+        <v>154</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="0"/>
-        <v>0.25840507734968382</v>
-      </c>
-      <c r="F33" t="s">
-        <v>153</v>
-      </c>
-      <c r="G33" t="s">
-        <v>154</v>
-      </c>
-      <c r="I33">
-        <f>255*E33</f>
         <v>65.89329472416938</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>20</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.24414062499999994</v>
+      </c>
+      <c r="F34" t="s">
+        <v>153</v>
+      </c>
+      <c r="G34" t="s">
+        <v>154</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="0"/>
-        <v>0.24414062499999994</v>
-      </c>
-      <c r="F34" t="s">
-        <v>153</v>
-      </c>
-      <c r="G34" t="s">
-        <v>154</v>
-      </c>
-      <c r="I34">
-        <f>255*E34</f>
         <v>62.255859374999986</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>21</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.23090704675198068</v>
+      </c>
+      <c r="F35" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" t="s">
+        <v>154</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="0"/>
-        <v>0.23090704675198068</v>
-      </c>
-      <c r="F35" t="s">
-        <v>153</v>
-      </c>
-      <c r="G35" t="s">
-        <v>154</v>
-      </c>
-      <c r="I35">
-        <f>255*E35</f>
         <v>58.881296921755073</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>22</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
+        <f t="shared" si="1"/>
+        <v>0.2186128750741097</v>
+      </c>
+      <c r="F36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" t="s">
+        <v>154</v>
+      </c>
+      <c r="I36">
         <f t="shared" si="0"/>
-        <v>0.2186128750741097</v>
-      </c>
-      <c r="F36" t="s">
-        <v>153</v>
-      </c>
-      <c r="G36" t="s">
-        <v>154</v>
-      </c>
-      <c r="I36">
-        <f>255*E36</f>
         <v>55.746283143897976</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>23</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
+        <f t="shared" si="1"/>
+        <v>0.20717621103300343</v>
+      </c>
+      <c r="F37" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" t="s">
+        <v>154</v>
+      </c>
+      <c r="I37">
         <f t="shared" si="0"/>
-        <v>0.20717621103300343</v>
-      </c>
-      <c r="F37" t="s">
-        <v>153</v>
-      </c>
-      <c r="G37" t="s">
-        <v>154</v>
-      </c>
-      <c r="I37">
-        <f>255*E37</f>
         <v>52.829933813415877</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>24</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="6">
+        <f t="shared" si="1"/>
+        <v>0.19652357654043043</v>
+      </c>
+      <c r="F38" t="s">
+        <v>153</v>
+      </c>
+      <c r="G38" t="s">
+        <v>154</v>
+      </c>
+      <c r="I38">
         <f t="shared" si="0"/>
-        <v>0.19652357654043043</v>
-      </c>
-      <c r="F38" t="s">
-        <v>153</v>
-      </c>
-      <c r="G38" t="s">
-        <v>154</v>
-      </c>
-      <c r="I38">
-        <f>255*E38</f>
         <v>50.113512017809761</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>25</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="6">
+        <f t="shared" si="1"/>
+        <v>0.18658892128279883</v>
+      </c>
+      <c r="F39" t="s">
+        <v>153</v>
+      </c>
+      <c r="G39" t="s">
+        <v>154</v>
+      </c>
+      <c r="I39">
         <f t="shared" si="0"/>
-        <v>0.18658892128279883</v>
-      </c>
-      <c r="F39" t="s">
-        <v>153</v>
-      </c>
-      <c r="G39" t="s">
-        <v>154</v>
-      </c>
-      <c r="I39">
-        <f>255*E39</f>
         <v>47.580174927113703</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>26</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="6">
+        <f t="shared" si="1"/>
+        <v>0.17731276127035372</v>
+      </c>
+      <c r="F40" t="s">
+        <v>153</v>
+      </c>
+      <c r="G40" t="s">
+        <v>154</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="0"/>
-        <v>0.17731276127035372</v>
-      </c>
-      <c r="F40" t="s">
-        <v>153</v>
-      </c>
-      <c r="G40" t="s">
-        <v>154</v>
-      </c>
-      <c r="I40">
-        <f>255*E40</f>
         <v>45.214754123940203</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>27</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="6">
+        <f t="shared" si="1"/>
+        <v>0.16864142970156706</v>
+      </c>
+      <c r="F41" t="s">
+        <v>153</v>
+      </c>
+      <c r="G41" t="s">
+        <v>154</v>
+      </c>
+      <c r="I41">
         <f t="shared" si="0"/>
-        <v>0.16864142970156706</v>
-      </c>
-      <c r="F41" t="s">
-        <v>153</v>
-      </c>
-      <c r="G41" t="s">
-        <v>154</v>
-      </c>
-      <c r="I41">
-        <f>255*E41</f>
         <v>43.003564573899602</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>28</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="6">
+        <f t="shared" si="1"/>
+        <v>0.16052642393359084</v>
+      </c>
+      <c r="F42" t="s">
+        <v>153</v>
+      </c>
+      <c r="G42" t="s">
+        <v>154</v>
+      </c>
+      <c r="I42">
         <f t="shared" si="0"/>
-        <v>0.16052642393359084</v>
-      </c>
-      <c r="F42" t="s">
-        <v>153</v>
-      </c>
-      <c r="G42" t="s">
-        <v>154</v>
-      </c>
-      <c r="I42">
-        <f>255*E42</f>
         <v>40.934238103065667</v>
       </c>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D43">
         <v>29</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="6">
+        <f t="shared" si="1"/>
+        <v>0.15292383490770972</v>
+      </c>
+      <c r="F43" t="s">
+        <v>153</v>
+      </c>
+      <c r="G43" t="s">
+        <v>154</v>
+      </c>
+      <c r="I43">
         <f t="shared" si="0"/>
-        <v>0.15292383490770972</v>
-      </c>
-      <c r="F43" t="s">
-        <v>153</v>
-      </c>
-      <c r="G43" t="s">
-        <v>154</v>
-      </c>
-      <c r="I43">
-        <f>255*E43</f>
         <v>38.995577901465978</v>
       </c>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D44">
         <v>30</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="6">
+        <f t="shared" si="1"/>
+        <v>0.14579384749963553</v>
+      </c>
+      <c r="F44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G44" t="s">
+        <v>154</v>
+      </c>
+      <c r="I44">
         <f t="shared" si="0"/>
-        <v>0.14579384749963553</v>
-      </c>
-      <c r="F44" t="s">
-        <v>153</v>
-      </c>
-      <c r="G44" t="s">
-        <v>154</v>
-      </c>
-      <c r="I44">
-        <f>255*E44</f>
         <v>37.177431112407064</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D45">
         <v>31</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="6">
+        <f t="shared" si="1"/>
+        <v>0.13910030202848581</v>
+      </c>
+      <c r="F45" t="s">
+        <v>153</v>
+      </c>
+      <c r="G45" t="s">
+        <v>154</v>
+      </c>
+      <c r="I45">
         <f t="shared" si="0"/>
-        <v>0.13910030202848581</v>
-      </c>
-      <c r="F45" t="s">
-        <v>153</v>
-      </c>
-      <c r="G45" t="s">
-        <v>154</v>
-      </c>
-      <c r="I45">
-        <f>255*E45</f>
         <v>35.470577017263878</v>
       </c>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D46">
         <v>32</v>
       </c>
-      <c r="E46" s="7">
-        <f t="shared" si="0"/>
+      <c r="E46" s="6">
+        <f t="shared" si="1"/>
         <v>0.13281030862990761</v>
       </c>
       <c r="F46" t="s">
@@ -2476,16 +2476,16 @@
         <v>154</v>
       </c>
       <c r="I46">
-        <f>255*E46</f>
+        <f t="shared" ref="I46:I77" si="2">255*E46</f>
         <v>33.866628700626443</v>
       </c>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D47">
         <v>33</v>
       </c>
-      <c r="E47" s="7">
-        <f t="shared" si="0"/>
+      <c r="E47" s="6">
+        <f t="shared" si="1"/>
         <v>0.12689390743013315</v>
       </c>
       <c r="F47" t="s">
@@ -2495,16 +2495,16 @@
         <v>154</v>
       </c>
       <c r="I47">
-        <f>255*E47</f>
+        <f t="shared" si="2"/>
         <v>32.357946394683957</v>
       </c>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D48">
         <v>34</v>
       </c>
-      <c r="E48" s="7">
-        <f t="shared" si="0"/>
+      <c r="E48" s="6">
+        <f t="shared" si="1"/>
         <v>0.12132376849095557</v>
       </c>
       <c r="F48" t="s">
@@ -2514,16 +2514,16 @@
         <v>154</v>
       </c>
       <c r="I48">
-        <f>255*E48</f>
+        <f t="shared" si="2"/>
         <v>30.937560965193668</v>
       </c>
     </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D49">
         <v>35</v>
       </c>
-      <c r="E49" s="7">
-        <f t="shared" si="0"/>
+      <c r="E49" s="6">
+        <f t="shared" si="1"/>
         <v>0.11607492636496861</v>
       </c>
       <c r="F49" t="s">
@@ -2533,16 +2533,16 @@
         <v>154</v>
       </c>
       <c r="I49">
-        <f>255*E49</f>
+        <f t="shared" si="2"/>
         <v>29.599106223066993</v>
       </c>
     </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D50">
         <v>36</v>
       </c>
-      <c r="E50" s="7">
-        <f t="shared" si="0"/>
+      <c r="E50" s="6">
+        <f t="shared" si="1"/>
         <v>0.11112454483386436</v>
       </c>
       <c r="F50" t="s">
@@ -2552,16 +2552,16 @@
         <v>154</v>
       </c>
       <c r="I50">
-        <f>255*E50</f>
+        <f t="shared" si="2"/>
         <v>28.336758932635412</v>
       </c>
     </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D51">
         <v>37</v>
       </c>
-      <c r="E51" s="7">
-        <f t="shared" si="0"/>
+      <c r="E51" s="6">
+        <f t="shared" si="1"/>
         <v>0.10645170802297783</v>
       </c>
       <c r="F51" t="s">
@@ -2571,16 +2571,16 @@
         <v>154</v>
       </c>
       <c r="I51">
-        <f>255*E51</f>
+        <f t="shared" si="2"/>
         <v>27.145185545859349</v>
       </c>
     </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D52">
         <v>38</v>
       </c>
-      <c r="E52" s="7">
-        <f t="shared" si="0"/>
+      <c r="E52" s="6">
+        <f t="shared" si="1"/>
         <v>0.10203723461135648</v>
       </c>
       <c r="F52" t="s">
@@ -2590,16 +2590,16 @@
         <v>154</v>
       </c>
       <c r="I52">
-        <f>255*E52</f>
+        <f t="shared" si="2"/>
         <v>26.019494825895904</v>
       </c>
     </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D53">
         <v>39</v>
       </c>
-      <c r="E53" s="7">
-        <f t="shared" si="0"/>
+      <c r="E53" s="6">
+        <f t="shared" si="1"/>
         <v>9.7863512303841146E-2</v>
       </c>
       <c r="F53" t="s">
@@ -2609,16 +2609,16 @@
         <v>154</v>
       </c>
       <c r="I53">
-        <f>255*E53</f>
+        <f t="shared" si="2"/>
         <v>24.955195637479491</v>
       </c>
     </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D54">
         <v>40</v>
       </c>
-      <c r="E54" s="7">
-        <f t="shared" si="0"/>
+      <c r="E54" s="6">
+        <f t="shared" si="1"/>
         <v>9.3914350112697192E-2</v>
       </c>
       <c r="F54" t="s">
@@ -2628,16 +2628,16 @@
         <v>154</v>
       </c>
       <c r="I54">
-        <f>255*E54</f>
+        <f t="shared" si="2"/>
         <v>23.948159278737783</v>
       </c>
     </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D55">
         <v>41</v>
       </c>
-      <c r="E55" s="7">
-        <f t="shared" si="0"/>
+      <c r="E55" s="6">
+        <f t="shared" si="1"/>
         <v>9.0174846321772528E-2</v>
       </c>
       <c r="F55" t="s">
@@ -2647,16 +2647,16 @@
         <v>154</v>
       </c>
       <c r="I55">
-        <f>255*E55</f>
+        <f t="shared" si="2"/>
         <v>22.994585812051994</v>
       </c>
     </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D56">
         <v>42</v>
       </c>
-      <c r="E56" s="7">
-        <f t="shared" si="0"/>
+      <c r="E56" s="6">
+        <f t="shared" si="1"/>
         <v>8.6631270284711973E-2</v>
       </c>
       <c r="F56" t="s">
@@ -2666,16 +2666,16 @@
         <v>154</v>
       </c>
       <c r="I56">
-        <f>255*E56</f>
+        <f t="shared" si="2"/>
         <v>22.090973922601552</v>
       </c>
     </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D57">
         <v>43</v>
       </c>
-      <c r="E57" s="7">
-        <f t="shared" si="0"/>
+      <c r="E57" s="6">
+        <f t="shared" si="1"/>
         <v>8.3270956447707614E-2</v>
       </c>
       <c r="F57" t="s">
@@ -2685,16 +2685,16 @@
         <v>154</v>
       </c>
       <c r="I57">
-        <f>255*E57</f>
+        <f t="shared" si="2"/>
         <v>21.23409389416544</v>
       </c>
     </row>
-    <row r="58" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D58">
         <v>44</v>
       </c>
-      <c r="E58" s="7">
-        <f t="shared" si="0"/>
+      <c r="E58" s="6">
+        <f t="shared" si="1"/>
         <v>8.0082209192668799E-2</v>
       </c>
       <c r="F58" t="s">
@@ -2704,16 +2704,16 @@
         <v>154</v>
       </c>
       <c r="I58">
-        <f>255*E58</f>
+        <f t="shared" si="2"/>
         <v>20.420963344130545</v>
       </c>
     </row>
-    <row r="59" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D59">
         <v>45</v>
       </c>
-      <c r="E59" s="7">
-        <f t="shared" si="0"/>
+      <c r="E59" s="6">
+        <f t="shared" si="1"/>
         <v>7.7054217273629141E-2</v>
       </c>
       <c r="F59" t="s">
@@ -2723,16 +2723,16 @@
         <v>154</v>
       </c>
       <c r="I59">
-        <f>255*E59</f>
+        <f t="shared" si="2"/>
         <v>19.64882540477543</v>
       </c>
     </row>
-    <row r="60" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D60">
         <v>46</v>
       </c>
-      <c r="E60" s="7">
-        <f t="shared" si="0"/>
+      <c r="E60" s="6">
+        <f t="shared" si="1"/>
         <v>7.4176976771924794E-2</v>
       </c>
       <c r="F60" t="s">
@@ -2742,16 +2742,16 @@
         <v>154</v>
       </c>
       <c r="I60">
-        <f>255*E60</f>
+        <f t="shared" si="2"/>
         <v>18.915129076840824</v>
       </c>
     </row>
-    <row r="61" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D61">
         <v>47</v>
       </c>
-      <c r="E61" s="7">
-        <f t="shared" si="0"/>
+      <c r="E61" s="6">
+        <f t="shared" si="1"/>
         <v>7.1441221627743925E-2</v>
       </c>
       <c r="F61" t="s">
@@ -2761,16 +2761,16 @@
         <v>154</v>
       </c>
       <c r="I61">
-        <f>255*E61</f>
+        <f t="shared" si="2"/>
         <v>18.217511515074701</v>
       </c>
     </row>
-    <row r="62" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D62">
         <v>48</v>
       </c>
-      <c r="E62" s="7">
-        <f t="shared" si="0"/>
+      <c r="E62" s="6">
+        <f t="shared" si="1"/>
         <v>6.8838360920077016E-2</v>
       </c>
       <c r="F62" t="s">
@@ -2780,16 +2780,16 @@
         <v>154</v>
       </c>
       <c r="I62">
-        <f>255*E62</f>
+        <f t="shared" si="2"/>
         <v>17.55378203461964</v>
       </c>
     </row>
-    <row r="63" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D63">
         <v>49</v>
       </c>
-      <c r="E63" s="7">
-        <f t="shared" si="0"/>
+      <c r="E63" s="6">
+        <f t="shared" si="1"/>
         <v>6.6360422166424932E-2</v>
       </c>
       <c r="F63" t="s">
@@ -2799,16 +2799,16 @@
         <v>154</v>
       </c>
       <c r="I63">
-        <f>255*E63</f>
+        <f t="shared" si="2"/>
         <v>16.921907652438357</v>
       </c>
     </row>
-    <row r="64" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D64">
         <v>50</v>
       </c>
-      <c r="E64" s="7">
-        <f t="shared" si="0"/>
+      <c r="E64" s="6">
+        <f t="shared" si="1"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="F64" t="s">
@@ -2818,16 +2818,16 @@
         <v>154</v>
       </c>
       <c r="I64">
-        <f>255*E64</f>
+        <f t="shared" si="2"/>
         <v>16.32</v>
       </c>
     </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D65">
         <v>51</v>
       </c>
-      <c r="E65" s="7">
-        <f t="shared" si="0"/>
+      <c r="E65" s="6">
+        <f t="shared" si="1"/>
         <v>6.175020965739933E-2</v>
       </c>
       <c r="F65" t="s">
@@ -2837,16 +2837,16 @@
         <v>154</v>
       </c>
       <c r="I65">
-        <f>255*E65</f>
+        <f t="shared" si="2"/>
         <v>15.746303462636829</v>
       </c>
     </row>
-    <row r="66" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D66">
         <v>52</v>
       </c>
-      <c r="E66" s="7">
-        <f t="shared" si="0"/>
+      <c r="E66" s="6">
+        <f t="shared" si="1"/>
         <v>5.9604644775390618E-2</v>
       </c>
       <c r="F66" t="s">
@@ -2856,16 +2856,16 @@
         <v>154</v>
       </c>
       <c r="I66">
-        <f>255*E66</f>
+        <f t="shared" si="2"/>
         <v>15.199184417724608</v>
       </c>
     </row>
-    <row r="67" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D67">
         <v>53</v>
       </c>
-      <c r="E67" s="7">
-        <f t="shared" si="0"/>
+      <c r="E67" s="6">
+        <f t="shared" si="1"/>
         <v>5.7557339052844506E-2</v>
       </c>
       <c r="F67" t="s">
@@ -2875,16 +2875,16 @@
         <v>154</v>
       </c>
       <c r="I67">
-        <f>255*E67</f>
+        <f t="shared" si="2"/>
         <v>14.67712145847535</v>
       </c>
     </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D68">
         <v>54</v>
       </c>
-      <c r="E68" s="7">
-        <f t="shared" si="0"/>
+      <c r="E68" s="6">
+        <f t="shared" si="1"/>
         <v>5.5602731384094314E-2</v>
       </c>
       <c r="F68" t="s">
@@ -2894,16 +2894,16 @@
         <v>154</v>
       </c>
       <c r="I68">
-        <f>255*E68</f>
+        <f t="shared" si="2"/>
         <v>14.178696502944049</v>
       </c>
     </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D69">
         <v>55</v>
       </c>
-      <c r="E69" s="7">
-        <f t="shared" si="0"/>
+      <c r="E69" s="6">
+        <f t="shared" si="1"/>
         <v>5.3735634114067295E-2</v>
       </c>
       <c r="F69" t="s">
@@ -2913,16 +2913,16 @@
         <v>154</v>
       </c>
       <c r="I69">
-        <f>255*E69</f>
+        <f t="shared" si="2"/>
         <v>13.70258669908716</v>
       </c>
     </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D70">
         <v>56</v>
       </c>
-      <c r="E70" s="7">
-        <f t="shared" si="0"/>
+      <c r="E70" s="6">
+        <f t="shared" si="1"/>
         <v>5.1951204104228238E-2</v>
       </c>
       <c r="F70" t="s">
@@ -2932,16 +2932,16 @@
         <v>154</v>
       </c>
       <c r="I70">
-        <f>255*E70</f>
+        <f t="shared" si="2"/>
         <v>13.247557046578201</v>
       </c>
     </row>
-    <row r="71" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D71">
         <v>57</v>
       </c>
-      <c r="E71" s="7">
-        <f t="shared" si="0"/>
+      <c r="E71" s="6">
+        <f t="shared" si="1"/>
         <v>5.0244916332416546E-2</v>
       </c>
       <c r="F71" t="s">
@@ -2951,16 +2951,16 @@
         <v>154</v>
       </c>
       <c r="I71">
-        <f>255*E71</f>
+        <f t="shared" si="2"/>
         <v>12.812453664766219</v>
       </c>
     </row>
-    <row r="72" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D72">
         <v>58</v>
       </c>
-      <c r="E72" s="7">
-        <f t="shared" si="0"/>
+      <c r="E72" s="6">
+        <f t="shared" si="1"/>
         <v>4.8612539779641313E-2</v>
       </c>
       <c r="F72" t="s">
@@ -2970,16 +2970,16 @@
         <v>154</v>
       </c>
       <c r="I72">
-        <f>255*E72</f>
+        <f t="shared" si="2"/>
         <v>12.396197643808534</v>
       </c>
     </row>
-    <row r="73" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D73">
         <v>59</v>
       </c>
-      <c r="E73" s="7">
-        <f t="shared" si="0"/>
+      <c r="E73" s="6">
+        <f t="shared" si="1"/>
         <v>4.7050115383350459E-2</v>
       </c>
       <c r="F73" t="s">
@@ -2989,16 +2989,16 @@
         <v>154</v>
       </c>
       <c r="I73">
-        <f>255*E73</f>
+        <f t="shared" si="2"/>
         <v>11.997779422754368</v>
       </c>
     </row>
-    <row r="74" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D74">
         <v>60</v>
       </c>
-      <c r="E74" s="7">
-        <f t="shared" si="0"/>
+      <c r="E74" s="6">
+        <f t="shared" si="1"/>
         <v>4.555393586005832E-2</v>
       </c>
       <c r="F74" t="s">
@@ -3008,16 +3008,16 @@
         <v>154</v>
       </c>
       <c r="I74">
-        <f>255*E74</f>
+        <f t="shared" si="2"/>
         <v>11.616253644314872</v>
       </c>
     </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D75">
         <v>61</v>
       </c>
-      <c r="E75" s="7">
-        <f t="shared" si="0"/>
+      <c r="E75" s="6">
+        <f t="shared" si="1"/>
         <v>4.4120527220887253E-2</v>
       </c>
       <c r="F75" t="s">
@@ -3027,16 +3027,16 @@
         <v>154</v>
       </c>
       <c r="I75">
-        <f>255*E75</f>
+        <f t="shared" si="2"/>
         <v>11.25073444132625</v>
       </c>
     </row>
-    <row r="76" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D76">
         <v>62</v>
       </c>
-      <c r="E76" s="7">
-        <f t="shared" si="0"/>
+      <c r="E76" s="6">
+        <f t="shared" si="1"/>
         <v>4.2746631821892235E-2</v>
       </c>
       <c r="F76" t="s">
@@ -3046,16 +3046,16 @@
         <v>154</v>
       </c>
       <c r="I76">
-        <f>255*E76</f>
+        <f t="shared" si="2"/>
         <v>10.90039111458252</v>
       </c>
     </row>
-    <row r="77" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D77">
         <v>63</v>
       </c>
-      <c r="E77" s="7">
-        <f t="shared" si="0"/>
+      <c r="E77" s="6">
+        <f t="shared" si="1"/>
         <v>4.1429192807278969E-2</v>
       </c>
       <c r="F77" t="s">
@@ -3065,16 +3065,16 @@
         <v>154</v>
       </c>
       <c r="I77">
-        <f>255*E77</f>
+        <f t="shared" si="2"/>
         <v>10.564444165856138</v>
       </c>
     </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D78">
         <v>64</v>
       </c>
-      <c r="E78" s="7">
-        <f t="shared" si="0"/>
+      <c r="E78" s="6">
+        <f t="shared" si="1"/>
         <v>4.016533981805423E-2</v>
       </c>
       <c r="F78" t="s">
@@ -3084,16 +3084,16 @@
         <v>154</v>
       </c>
       <c r="I78">
-        <f>255*E78</f>
+        <f t="shared" ref="I78:I109" si="3">255*E78</f>
         <v>10.242161653603828</v>
       </c>
     </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D79">
         <v>65</v>
       </c>
-      <c r="E79" s="7">
-        <f t="shared" ref="E79:E142" si="1">1/(((D79/100*3)+1)^3)</f>
+      <c r="E79" s="6">
+        <f t="shared" ref="E79:E142" si="4">1/(((D79/100*3)+1)^3)</f>
         <v>3.895237585147459E-2</v>
       </c>
       <c r="F79" t="s">
@@ -3103,16 +3103,16 @@
         <v>154</v>
       </c>
       <c r="I79">
-        <f>255*E79</f>
+        <f t="shared" si="3"/>
         <v>9.9328558421260205</v>
       </c>
     </row>
-    <row r="80" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D80">
         <v>66</v>
       </c>
-      <c r="E80" s="7">
-        <f t="shared" si="1"/>
+      <c r="E80" s="6">
+        <f t="shared" si="4"/>
         <v>3.7787765168084519E-2</v>
       </c>
       <c r="F80" t="s">
@@ -3122,16 +3122,16 @@
         <v>154</v>
       </c>
       <c r="I80">
-        <f>255*E80</f>
+        <f t="shared" si="3"/>
         <v>9.6358801178615519</v>
       </c>
     </row>
-    <row r="81" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D81">
         <v>67</v>
       </c>
-      <c r="E81" s="7">
-        <f t="shared" si="1"/>
+      <c r="E81" s="6">
+        <f t="shared" si="4"/>
         <v>3.6669122153316448E-2</v>
       </c>
       <c r="F81" t="s">
@@ -3141,16 +3141,16 @@
         <v>154</v>
       </c>
       <c r="I81">
-        <f>255*E81</f>
+        <f t="shared" si="3"/>
         <v>9.3506261490956941</v>
       </c>
     </row>
-    <row r="82" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D82">
         <v>68</v>
       </c>
-      <c r="E82" s="7">
-        <f t="shared" si="1"/>
+      <c r="E82" s="6">
+        <f t="shared" si="4"/>
         <v>3.5594201049715703E-2</v>
       </c>
       <c r="F82" t="s">
@@ -3160,16 +3160,16 @@
         <v>154</v>
       </c>
       <c r="I82">
-        <f>255*E82</f>
+        <f t="shared" si="3"/>
         <v>9.0765212676775047</v>
       </c>
     </row>
-    <row r="83" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D83">
         <v>69</v>
       </c>
-      <c r="E83" s="7">
-        <f t="shared" si="1"/>
+      <c r="E83" s="6">
+        <f t="shared" si="4"/>
         <v>3.4560886483973451E-2</v>
       </c>
       <c r="F83" t="s">
@@ -3179,16 +3179,16 @@
         <v>154</v>
       </c>
       <c r="I83">
-        <f>255*E83</f>
+        <f t="shared" si="3"/>
         <v>8.8130260534132301</v>
       </c>
     </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D84">
         <v>70</v>
       </c>
-      <c r="E84" s="7">
-        <f t="shared" si="1"/>
+      <c r="E84" s="6">
+        <f t="shared" si="4"/>
         <v>3.3567184720217524E-2</v>
       </c>
       <c r="F84" t="s">
@@ -3198,16 +3198,16 @@
         <v>154</v>
       </c>
       <c r="I84">
-        <f>255*E84</f>
+        <f t="shared" si="3"/>
         <v>8.5596321036554688</v>
       </c>
     </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D85">
         <v>71</v>
       </c>
-      <c r="E85" s="7">
-        <f t="shared" si="1"/>
+      <c r="E85" s="6">
+        <f t="shared" si="4"/>
         <v>3.2611215577516749E-2</v>
       </c>
       <c r="F85" t="s">
@@ -3217,16 +3217,16 @@
         <v>154</v>
       </c>
       <c r="I85">
-        <f>255*E85</f>
+        <f t="shared" si="3"/>
         <v>8.3158599722667716</v>
       </c>
     </row>
-    <row r="86" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D86">
         <v>72</v>
       </c>
-      <c r="E86" s="7">
-        <f t="shared" si="1"/>
+      <c r="E86" s="6">
+        <f t="shared" si="4"/>
         <v>3.1691204955388914E-2</v>
       </c>
       <c r="F86" t="s">
@@ -3236,16 +3236,16 @@
         <v>154</v>
       </c>
       <c r="I86">
-        <f>255*E86</f>
+        <f t="shared" si="3"/>
         <v>8.081257263624174</v>
       </c>
     </row>
-    <row r="87" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D87">
         <v>73</v>
       </c>
-      <c r="E87" s="7">
-        <f t="shared" si="1"/>
+      <c r="E87" s="6">
+        <f t="shared" si="4"/>
         <v>3.080547791633842E-2</v>
       </c>
       <c r="F87" t="s">
@@ -3255,16 +3255,16 @@
         <v>154</v>
       </c>
       <c r="I87">
-        <f>255*E87</f>
+        <f t="shared" si="3"/>
         <v>7.8553968686662969</v>
       </c>
     </row>
-    <row r="88" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D88">
         <v>74</v>
       </c>
-      <c r="E88" s="7">
-        <f t="shared" si="1"/>
+      <c r="E88" s="6">
+        <f t="shared" si="4"/>
         <v>2.9952452279153993E-2</v>
       </c>
       <c r="F88" t="s">
@@ -3274,16 +3274,16 @@
         <v>154</v>
       </c>
       <c r="I88">
-        <f>255*E88</f>
+        <f t="shared" si="3"/>
         <v>7.6378753311842678</v>
       </c>
     </row>
-    <row r="89" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D89">
         <v>75</v>
       </c>
-      <c r="E89" s="7">
-        <f t="shared" si="1"/>
+      <c r="E89" s="6">
+        <f t="shared" si="4"/>
         <v>2.9130632680928539E-2</v>
       </c>
       <c r="F89" t="s">
@@ -3293,16 +3293,16 @@
         <v>154</v>
       </c>
       <c r="I89">
-        <f>255*E89</f>
+        <f t="shared" si="3"/>
         <v>7.4283113336367776</v>
       </c>
     </row>
-    <row r="90" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D90">
         <v>76</v>
       </c>
-      <c r="E90" s="7">
-        <f t="shared" si="1"/>
+      <c r="E90" s="6">
+        <f t="shared" si="4"/>
         <v>2.8338605069572406E-2</v>
       </c>
       <c r="F90" t="s">
@@ -3312,16 +3312,16 @@
         <v>154</v>
       </c>
       <c r="I90">
-        <f>255*E90</f>
+        <f t="shared" si="3"/>
         <v>7.226344292740964</v>
       </c>
     </row>
-    <row r="91" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D91">
         <v>77</v>
       </c>
-      <c r="E91" s="7">
-        <f t="shared" si="1"/>
+      <c r="E91" s="6">
+        <f t="shared" si="4"/>
         <v>2.7575031592024315E-2</v>
       </c>
       <c r="F91" t="s">
@@ -3331,16 +3331,16 @@
         <v>154</v>
       </c>
       <c r="I91">
-        <f>255*E91</f>
+        <f t="shared" si="3"/>
         <v>7.0316330559661999</v>
       </c>
     </row>
-    <row r="92" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D92">
         <v>78</v>
       </c>
-      <c r="E92" s="7">
-        <f t="shared" si="1"/>
+      <c r="E92" s="6">
+        <f t="shared" si="4"/>
         <v>2.6838645846461905E-2</v>
       </c>
       <c r="F92" t="s">
@@ -3350,16 +3350,16 @@
         <v>154</v>
       </c>
       <c r="I92">
-        <f>255*E92</f>
+        <f t="shared" si="3"/>
         <v>6.8438546908477855</v>
       </c>
     </row>
-    <row r="93" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D93">
         <v>79</v>
       </c>
-      <c r="E93" s="7">
-        <f t="shared" si="1"/>
+      <c r="E93" s="6">
+        <f t="shared" si="4"/>
         <v>2.6128248469609691E-2</v>
       </c>
       <c r="F93" t="s">
@@ -3369,16 +3369,16 @@
         <v>154</v>
       </c>
       <c r="I93">
-        <f>255*E93</f>
+        <f t="shared" si="3"/>
         <v>6.6627033597504717</v>
       </c>
     </row>
-    <row r="94" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D94">
         <v>80</v>
       </c>
-      <c r="E94" s="7">
-        <f t="shared" si="1"/>
+      <c r="E94" s="6">
+        <f t="shared" si="4"/>
         <v>2.5442703032770197E-2</v>
       </c>
       <c r="F94" t="s">
@@ -3388,16 +3388,16 @@
         <v>154</v>
       </c>
       <c r="I94">
-        <f>255*E94</f>
+        <f t="shared" si="3"/>
         <v>6.4878892733563998</v>
       </c>
     </row>
-    <row r="95" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D95">
         <v>81</v>
       </c>
-      <c r="E95" s="7">
-        <f t="shared" si="1"/>
+      <c r="E95" s="6">
+        <f t="shared" si="4"/>
         <v>2.4780932222490046E-2</v>
       </c>
       <c r="F95" t="s">
@@ -3407,16 +3407,16 @@
         <v>154</v>
       </c>
       <c r="I95">
-        <f>255*E95</f>
+        <f t="shared" si="3"/>
         <v>6.3191377167349616</v>
       </c>
     </row>
-    <row r="96" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D96">
         <v>82</v>
       </c>
-      <c r="E96" s="7">
-        <f t="shared" si="1"/>
+      <c r="E96" s="6">
+        <f t="shared" si="4"/>
         <v>2.414191428384363E-2</v>
       </c>
       <c r="F96" t="s">
@@ -3426,16 +3426,16 @@
         <v>154</v>
       </c>
       <c r="I96">
-        <f>255*E96</f>
+        <f t="shared" si="3"/>
         <v>6.1561881423801257</v>
       </c>
     </row>
-    <row r="97" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D97">
         <v>83</v>
       </c>
-      <c r="E97" s="7">
-        <f t="shared" si="1"/>
+      <c r="E97" s="6">
+        <f t="shared" si="4"/>
         <v>2.3524679706192753E-2</v>
       </c>
       <c r="F97" t="s">
@@ -3445,16 +3445,16 @@
         <v>154</v>
       </c>
       <c r="I97">
-        <f>255*E97</f>
+        <f t="shared" si="3"/>
         <v>5.9987933250791521</v>
       </c>
     </row>
-    <row r="98" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D98">
         <v>84</v>
       </c>
-      <c r="E98" s="7">
-        <f t="shared" si="1"/>
+      <c r="E98" s="6">
+        <f t="shared" si="4"/>
         <v>2.292830813298272E-2</v>
       </c>
       <c r="F98" t="s">
@@ -3464,16 +3464,16 @@
         <v>154</v>
       </c>
       <c r="I98">
-        <f>255*E98</f>
+        <f t="shared" si="3"/>
         <v>5.8467185739105938</v>
       </c>
     </row>
-    <row r="99" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D99">
         <v>85</v>
       </c>
-      <c r="E99" s="7">
-        <f t="shared" si="1"/>
+      <c r="E99" s="6">
+        <f t="shared" si="4"/>
         <v>2.2351925478680458E-2</v>
       </c>
       <c r="F99" t="s">
@@ -3483,16 +3483,16 @@
         <v>154</v>
       </c>
       <c r="I99">
-        <f>255*E99</f>
+        <f t="shared" si="3"/>
         <v>5.6997409970635164</v>
       </c>
     </row>
-    <row r="100" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D100">
         <v>86</v>
       </c>
-      <c r="E100" s="7">
-        <f t="shared" si="1"/>
+      <c r="E100" s="6">
+        <f t="shared" si="4"/>
         <v>2.1794701237363653E-2</v>
       </c>
       <c r="F100" t="s">
@@ -3502,16 +3502,16 @@
         <v>154</v>
       </c>
       <c r="I100">
-        <f>255*E100</f>
+        <f t="shared" si="3"/>
         <v>5.557648815527731</v>
       </c>
     </row>
-    <row r="101" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D101">
         <v>87</v>
       </c>
-      <c r="E101" s="7">
-        <f t="shared" si="1"/>
+      <c r="E101" s="6">
+        <f t="shared" si="4"/>
         <v>2.1255845968746981E-2</v>
       </c>
       <c r="F101" t="s">
@@ -3521,16 +3521,16 @@
         <v>154</v>
       </c>
       <c r="I101">
-        <f>255*E101</f>
+        <f t="shared" si="3"/>
         <v>5.4202407220304805</v>
       </c>
     </row>
-    <row r="102" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D102">
         <v>88</v>
       </c>
-      <c r="E102" s="7">
-        <f t="shared" si="1"/>
+      <c r="E102" s="6">
+        <f t="shared" si="4"/>
         <v>2.0734608948592765E-2</v>
       </c>
       <c r="F102" t="s">
@@ -3540,16 +3540,16 @@
         <v>154</v>
       </c>
       <c r="I102">
-        <f>255*E102</f>
+        <f t="shared" si="3"/>
         <v>5.2873252818911549</v>
       </c>
     </row>
-    <row r="103" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D103">
         <v>89</v>
       </c>
-      <c r="E103" s="7">
-        <f t="shared" si="1"/>
+      <c r="E103" s="6">
+        <f t="shared" si="4"/>
         <v>2.0230275971511971E-2</v>
       </c>
       <c r="F103" t="s">
@@ -3559,16 +3559,16 @@
         <v>154</v>
       </c>
       <c r="I103">
-        <f>255*E103</f>
+        <f t="shared" si="3"/>
         <v>5.1587203727355524</v>
       </c>
     </row>
-    <row r="104" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D104">
         <v>90</v>
       </c>
-      <c r="E104" s="7">
-        <f t="shared" si="1"/>
+      <c r="E104" s="6">
+        <f t="shared" si="4"/>
         <v>1.9742167295125658E-2</v>
       </c>
       <c r="F104" t="s">
@@ -3578,16 +3578,16 @@
         <v>154</v>
       </c>
       <c r="I104">
-        <f>255*E104</f>
+        <f t="shared" si="3"/>
         <v>5.0342526602570432</v>
       </c>
     </row>
-    <row r="105" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D105">
         <v>91</v>
       </c>
-      <c r="E105" s="7">
-        <f t="shared" si="1"/>
+      <c r="E105" s="6">
+        <f t="shared" si="4"/>
         <v>1.9269635715437352E-2</v>
       </c>
       <c r="F105" t="s">
@@ -3597,16 +3597,16 @@
         <v>154</v>
       </c>
       <c r="I105">
-        <f>255*E105</f>
+        <f t="shared" si="3"/>
         <v>4.9137571074365249</v>
       </c>
     </row>
-    <row r="106" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D106">
         <v>92</v>
       </c>
-      <c r="E106" s="7">
-        <f t="shared" si="1"/>
+      <c r="E106" s="6">
+        <f t="shared" si="4"/>
         <v>1.8812064764069613E-2</v>
       </c>
       <c r="F106" t="s">
@@ -3616,16 +3616,16 @@
         <v>154</v>
       </c>
       <c r="I106">
-        <f>255*E106</f>
+        <f t="shared" si="3"/>
         <v>4.7970765148377517</v>
       </c>
     </row>
-    <row r="107" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D107">
         <v>93</v>
       </c>
-      <c r="E107" s="7">
-        <f t="shared" si="1"/>
+      <c r="E107" s="6">
+        <f t="shared" si="4"/>
         <v>1.8368867018752538E-2</v>
       </c>
       <c r="F107" t="s">
@@ -3635,16 +3635,16 @@
         <v>154</v>
       </c>
       <c r="I107">
-        <f>255*E107</f>
+        <f t="shared" si="3"/>
         <v>4.6840610897818973</v>
       </c>
     </row>
-    <row r="108" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D108">
         <v>94</v>
       </c>
-      <c r="E108" s="7">
-        <f t="shared" si="1"/>
+      <c r="E108" s="6">
+        <f t="shared" si="4"/>
         <v>1.7939482519122411E-2</v>
       </c>
       <c r="F108" t="s">
@@ -3654,16 +3654,16 @@
         <v>154</v>
       </c>
       <c r="I108">
-        <f>255*E108</f>
+        <f t="shared" si="3"/>
         <v>4.5745680423762147</v>
       </c>
     </row>
-    <row r="109" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D109">
         <v>95</v>
       </c>
-      <c r="E109" s="7">
-        <f t="shared" si="1"/>
+      <c r="E109" s="6">
+        <f t="shared" si="4"/>
         <v>1.7523377280503277E-2</v>
       </c>
       <c r="F109" t="s">
@@ -3673,16 +3673,16 @@
         <v>154</v>
       </c>
       <c r="I109">
-        <f>255*E109</f>
+        <f t="shared" si="3"/>
         <v>4.4684612065283353</v>
       </c>
     </row>
-    <row r="110" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D110">
         <v>96</v>
       </c>
-      <c r="E110" s="7">
-        <f t="shared" si="1"/>
+      <c r="E110" s="6">
+        <f t="shared" si="4"/>
         <v>1.7120041898905744E-2</v>
       </c>
       <c r="F110" t="s">
@@ -3692,16 +3692,16 @@
         <v>154</v>
       </c>
       <c r="I110">
-        <f>255*E110</f>
+        <f t="shared" ref="I110:I141" si="5">255*E110</f>
         <v>4.3656106842209645</v>
       </c>
     </row>
-    <row r="111" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D111">
         <v>97</v>
       </c>
-      <c r="E111" s="7">
-        <f t="shared" si="1"/>
+      <c r="E111" s="6">
+        <f t="shared" si="4"/>
         <v>1.6728990240992978E-2</v>
       </c>
       <c r="F111" t="s">
@@ -3711,16 +3711,16 @@
         <v>154</v>
       </c>
       <c r="I111">
-        <f>255*E111</f>
+        <f t="shared" si="5"/>
         <v>4.2658925114532096</v>
       </c>
     </row>
-    <row r="112" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D112">
         <v>98</v>
       </c>
-      <c r="E112" s="7">
-        <f t="shared" si="1"/>
+      <c r="E112" s="6">
+        <f t="shared" si="4"/>
         <v>1.634975821323564E-2</v>
       </c>
       <c r="F112" t="s">
@@ -3730,16 +3730,16 @@
         <v>154</v>
       </c>
       <c r="I112">
-        <f>255*E112</f>
+        <f t="shared" si="5"/>
         <v>4.1691883443750886</v>
       </c>
     </row>
-    <row r="113" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D113">
         <v>99</v>
       </c>
-      <c r="E113" s="7">
-        <f t="shared" si="1"/>
+      <c r="E113" s="6">
+        <f t="shared" si="4"/>
         <v>1.5981902604911086E-2</v>
       </c>
       <c r="F113" t="s">
@@ -3749,16 +3749,16 @@
         <v>154</v>
       </c>
       <c r="I113">
-        <f>255*E113</f>
+        <f t="shared" si="5"/>
         <v>4.0753851642523271</v>
       </c>
     </row>
-    <row r="114" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D114">
         <v>100</v>
       </c>
-      <c r="E114" s="7">
-        <f t="shared" si="1"/>
+      <c r="E114" s="6">
+        <f t="shared" si="4"/>
         <v>1.5625E-2</v>
       </c>
       <c r="F114" t="s">
@@ -3768,16 +3768,16 @@
         <v>154</v>
       </c>
       <c r="I114">
-        <f>255*E114</f>
+        <f t="shared" si="5"/>
         <v>3.984375</v>
       </c>
     </row>
-    <row r="115" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D115">
         <v>101</v>
       </c>
-      <c r="E115" s="7">
-        <f t="shared" si="1"/>
+      <c r="E115" s="6">
+        <f t="shared" si="4"/>
         <v>1.5278645753398956E-2</v>
       </c>
       <c r="F115" t="s">
@@ -3787,16 +3787,16 @@
         <v>154</v>
       </c>
       <c r="I115">
-        <f>255*E115</f>
+        <f t="shared" si="5"/>
         <v>3.8960546671167338</v>
       </c>
     </row>
-    <row r="116" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D116">
         <v>102</v>
       </c>
-      <c r="E116" s="7">
-        <f t="shared" si="1"/>
+      <c r="E116" s="6">
+        <f t="shared" si="4"/>
         <v>1.4942453027203508E-2</v>
       </c>
       <c r="F116" t="s">
@@ -3806,16 +3806,16 @@
         <v>154</v>
       </c>
       <c r="I116">
-        <f>255*E116</f>
+        <f t="shared" si="5"/>
         <v>3.8103255219368948</v>
       </c>
     </row>
-    <row r="117" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D117">
         <v>103</v>
       </c>
-      <c r="E117" s="7">
-        <f t="shared" si="1"/>
+      <c r="E117" s="6">
+        <f t="shared" si="4"/>
         <v>1.461605188312555E-2</v>
       </c>
       <c r="F117" t="s">
@@ -3825,16 +3825,16 @@
         <v>154</v>
       </c>
       <c r="I117">
-        <f>255*E117</f>
+        <f t="shared" si="5"/>
         <v>3.7270932301970152</v>
       </c>
     </row>
-    <row r="118" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D118">
         <v>104</v>
       </c>
-      <c r="E118" s="7">
-        <f t="shared" si="1"/>
+      <c r="E118" s="6">
+        <f t="shared" si="4"/>
         <v>1.4299088427393119E-2</v>
       </c>
       <c r="F118" t="s">
@@ -3844,16 +3844,16 @@
         <v>154</v>
       </c>
       <c r="I118">
-        <f>255*E118</f>
+        <f t="shared" si="5"/>
         <v>3.6462675489852452</v>
       </c>
     </row>
-    <row r="119" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D119">
         <v>105</v>
       </c>
-      <c r="E119" s="7">
-        <f t="shared" si="1"/>
+      <c r="E119" s="6">
+        <f t="shared" si="4"/>
         <v>1.3991224004743022E-2</v>
       </c>
       <c r="F119" t="s">
@@ -3863,16 +3863,16 @@
         <v>154</v>
       </c>
       <c r="I119">
-        <f>255*E119</f>
+        <f t="shared" si="5"/>
         <v>3.5677621212094706</v>
       </c>
     </row>
-    <row r="120" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D120">
         <v>106</v>
       </c>
-      <c r="E120" s="7">
-        <f t="shared" si="1"/>
+      <c r="E120" s="6">
+        <f t="shared" si="4"/>
         <v>1.3692134438357957E-2</v>
       </c>
       <c r="F120" t="s">
@@ -3882,16 +3882,16 @@
         <v>154</v>
       </c>
       <c r="I120">
-        <f>255*E120</f>
+        <f t="shared" si="5"/>
         <v>3.4914942817812791</v>
       </c>
     </row>
-    <row r="121" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D121">
         <v>107</v>
       </c>
-      <c r="E121" s="7">
-        <f t="shared" si="1"/>
+      <c r="E121" s="6">
+        <f t="shared" si="4"/>
         <v>1.3401509312822735E-2</v>
       </c>
       <c r="F121" t="s">
@@ -3901,16 +3901,16 @@
         <v>154</v>
       </c>
       <c r="I121">
-        <f>255*E121</f>
+        <f t="shared" si="5"/>
         <v>3.4173848747697977</v>
       </c>
     </row>
-    <row r="122" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D122">
         <v>108</v>
       </c>
-      <c r="E122" s="7">
-        <f t="shared" si="1"/>
+      <c r="E122" s="6">
+        <f t="shared" si="4"/>
         <v>1.3119051297379712E-2</v>
       </c>
       <c r="F122" t="s">
@@ -3920,16 +3920,16 @@
         <v>154</v>
       </c>
       <c r="I122">
-        <f>255*E122</f>
+        <f t="shared" si="5"/>
         <v>3.3453580808318266</v>
       </c>
     </row>
-    <row r="123" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D123">
         <v>109</v>
       </c>
-      <c r="E123" s="7">
-        <f t="shared" si="1"/>
+      <c r="E123" s="6">
+        <f t="shared" si="4"/>
         <v>1.284447550695314E-2</v>
       </c>
       <c r="F123" t="s">
@@ -3939,16 +3939,16 @@
         <v>154</v>
       </c>
       <c r="I123">
-        <f>255*E123</f>
+        <f t="shared" si="5"/>
         <v>3.2753412542730507</v>
       </c>
     </row>
-    <row r="124" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D124">
         <v>110</v>
       </c>
-      <c r="E124" s="7">
-        <f t="shared" si="1"/>
+      <c r="E124" s="6">
+        <f t="shared" si="4"/>
         <v>1.2577508898587541E-2</v>
       </c>
       <c r="F124" t="s">
@@ -3958,16 +3958,16 @@
         <v>154</v>
       </c>
       <c r="I124">
-        <f>255*E124</f>
+        <f t="shared" si="5"/>
         <v>3.2072647691398228</v>
       </c>
     </row>
-    <row r="125" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D125">
         <v>111</v>
       </c>
-      <c r="E125" s="7">
-        <f t="shared" si="1"/>
+      <c r="E125" s="6">
+        <f t="shared" si="4"/>
         <v>1.2317889701107268E-2</v>
       </c>
       <c r="F125" t="s">
@@ -3977,16 +3977,16 @@
         <v>154</v>
       </c>
       <c r="I125">
-        <f>255*E125</f>
+        <f t="shared" si="5"/>
         <v>3.1410618737823532</v>
       </c>
     </row>
-    <row r="126" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D126">
         <v>112</v>
       </c>
-      <c r="E126" s="7">
-        <f t="shared" si="1"/>
+      <c r="E126" s="6">
+        <f t="shared" si="4"/>
         <v>1.2065366875954128E-2</v>
       </c>
       <c r="F126" t="s">
@@ -3996,16 +3996,16 @@
         <v>154</v>
       </c>
       <c r="I126">
-        <f>255*E126</f>
+        <f t="shared" si="5"/>
         <v>3.0766685533683025</v>
       </c>
     </row>
-    <row r="127" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D127">
         <v>113</v>
       </c>
-      <c r="E127" s="7">
-        <f t="shared" si="1"/>
+      <c r="E127" s="6">
+        <f t="shared" si="4"/>
         <v>1.1819699607298758E-2</v>
       </c>
       <c r="F127" t="s">
@@ -4015,16 +4015,16 @@
         <v>154</v>
       </c>
       <c r="I127">
-        <f>255*E127</f>
+        <f t="shared" si="5"/>
         <v>3.0140233998611832</v>
       </c>
     </row>
-    <row r="128" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D128">
         <v>114</v>
       </c>
-      <c r="E128" s="7">
-        <f t="shared" si="1"/>
+      <c r="E128" s="6">
+        <f t="shared" si="4"/>
         <v>1.1580656819649614E-2</v>
       </c>
       <c r="F128" t="s">
@@ -4034,16 +4034,16 @@
         <v>154</v>
       </c>
       <c r="I128">
-        <f>255*E128</f>
+        <f t="shared" si="5"/>
         <v>2.9530674890106514</v>
       </c>
     </row>
-    <row r="129" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D129">
         <v>115</v>
       </c>
-      <c r="E129" s="7">
-        <f t="shared" si="1"/>
+      <c r="E129" s="6">
+        <f t="shared" si="4"/>
         <v>1.1348016721302643E-2</v>
       </c>
       <c r="F129" t="s">
@@ -4053,16 +4053,16 @@
         <v>154</v>
       </c>
       <c r="I129">
-        <f>255*E129</f>
+        <f t="shared" si="5"/>
         <v>2.8937442639321742</v>
       </c>
     </row>
-    <row r="130" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D130">
         <v>116</v>
       </c>
-      <c r="E130" s="7">
-        <f t="shared" si="1"/>
+      <c r="E130" s="6">
+        <f t="shared" si="4"/>
         <v>1.1121566372084552E-2</v>
       </c>
       <c r="F130" t="s">
@@ -4072,16 +4072,16 @@
         <v>154</v>
       </c>
       <c r="I130">
-        <f>255*E130</f>
+        <f t="shared" si="5"/>
         <v>2.8359994248815608</v>
       </c>
     </row>
-    <row r="131" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D131">
         <v>117</v>
       </c>
-      <c r="E131" s="7">
-        <f t="shared" si="1"/>
+      <c r="E131" s="6">
+        <f t="shared" si="4"/>
         <v>1.090110127394521E-2</v>
       </c>
       <c r="F131" t="s">
@@ -4091,16 +4091,16 @@
         <v>154</v>
       </c>
       <c r="I131">
-        <f>255*E131</f>
+        <f t="shared" si="5"/>
         <v>2.7797808248560285</v>
       </c>
     </row>
-    <row r="132" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D132">
         <v>118</v>
       </c>
-      <c r="E132" s="7">
-        <f t="shared" si="1"/>
+      <c r="E132" s="6">
+        <f t="shared" si="4"/>
         <v>1.0686424983049194E-2</v>
       </c>
       <c r="F132" t="s">
@@ -4110,16 +4110,16 @@
         <v>154</v>
       </c>
       <c r="I132">
-        <f>255*E132</f>
+        <f t="shared" si="5"/>
         <v>2.7250383706775443</v>
       </c>
     </row>
-    <row r="133" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D133">
         <v>119</v>
       </c>
-      <c r="E133" s="7">
-        <f t="shared" si="1"/>
+      <c r="E133" s="6">
+        <f t="shared" si="4"/>
         <v>1.04773487421047E-2</v>
       </c>
       <c r="F133" t="s">
@@ -4129,16 +4129,16 @@
         <v>154</v>
       </c>
       <c r="I133">
-        <f>255*E133</f>
+        <f t="shared" si="5"/>
         <v>2.6717239292366983</v>
       </c>
     </row>
-    <row r="134" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D134">
         <v>120</v>
       </c>
-      <c r="E134" s="7">
-        <f t="shared" si="1"/>
+      <c r="E134" s="6">
+        <f t="shared" si="4"/>
         <v>1.0273691131749817E-2</v>
       </c>
       <c r="F134" t="s">
@@ -4148,16 +4148,16 @@
         <v>154</v>
       </c>
       <c r="I134">
-        <f>255*E134</f>
+        <f t="shared" si="5"/>
         <v>2.6197912385962034</v>
       </c>
     </row>
-    <row r="135" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D135">
         <v>121</v>
       </c>
-      <c r="E135" s="7">
-        <f t="shared" si="1"/>
+      <c r="E135" s="6">
+        <f t="shared" si="4"/>
         <v>1.0075277739891936E-2</v>
       </c>
       <c r="F135" t="s">
@@ -4167,16 +4167,16 @@
         <v>154</v>
       </c>
       <c r="I135">
-        <f>255*E135</f>
+        <f t="shared" si="5"/>
         <v>2.5691958236724437</v>
       </c>
     </row>
-    <row r="136" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D136">
         <v>122</v>
       </c>
-      <c r="E136" s="7">
-        <f t="shared" si="1"/>
+      <c r="E136" s="6">
+        <f t="shared" si="4"/>
         <v>9.8819408479669715E-3</v>
       </c>
       <c r="F136" t="s">
@@ -4186,16 +4186,16 @@
         <v>154</v>
       </c>
       <c r="I136">
-        <f>255*E136</f>
+        <f t="shared" si="5"/>
         <v>2.5198949162315776</v>
       </c>
     </row>
-    <row r="137" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D137">
         <v>123</v>
       </c>
-      <c r="E137" s="7">
-        <f t="shared" si="1"/>
+      <c r="E137" s="6">
+        <f t="shared" si="4"/>
         <v>9.693519133150464E-3</v>
       </c>
       <c r="F137" t="s">
@@ -4205,16 +4205,16 @@
         <v>154</v>
       </c>
       <c r="I137">
-        <f>255*E137</f>
+        <f t="shared" si="5"/>
         <v>2.4718473789533681</v>
       </c>
     </row>
-    <row r="138" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D138">
         <v>124</v>
       </c>
-      <c r="E138" s="7">
-        <f t="shared" si="1"/>
+      <c r="E138" s="6">
+        <f t="shared" si="4"/>
         <v>9.5098573856139141E-3</v>
       </c>
       <c r="F138" t="s">
@@ -4224,16 +4224,16 @@
         <v>154</v>
       </c>
       <c r="I138">
-        <f>255*E138</f>
+        <f t="shared" si="5"/>
         <v>2.425013633331548</v>
       </c>
     </row>
-    <row r="139" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D139">
         <v>125</v>
       </c>
-      <c r="E139" s="7">
-        <f t="shared" si="1"/>
+      <c r="E139" s="6">
+        <f t="shared" si="4"/>
         <v>9.3308062399766727E-3</v>
       </c>
       <c r="F139" t="s">
@@ -4243,16 +4243,16 @@
         <v>154</v>
       </c>
       <c r="I139">
-        <f>255*E139</f>
+        <f t="shared" si="5"/>
         <v>2.3793555911940514</v>
       </c>
     </row>
-    <row r="140" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D140">
         <v>126</v>
       </c>
-      <c r="E140" s="7">
-        <f t="shared" si="1"/>
+      <c r="E140" s="6">
+        <f t="shared" si="4"/>
         <v>9.1562219201564259E-3</v>
       </c>
       <c r="F140" t="s">
@@ -4262,16 +4262,16 @@
         <v>154</v>
       </c>
       <c r="I140">
-        <f>255*E140</f>
+        <f t="shared" si="5"/>
         <v>2.3348365896398886</v>
       </c>
     </row>
-    <row r="141" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D141">
         <v>127</v>
       </c>
-      <c r="E141" s="7">
-        <f t="shared" si="1"/>
+      <c r="E141" s="6">
+        <f t="shared" si="4"/>
         <v>8.9859659968710304E-3</v>
       </c>
       <c r="F141" t="s">
@@ -4281,16 +4281,16 @@
         <v>154</v>
       </c>
       <c r="I141">
-        <f>255*E141</f>
+        <f t="shared" si="5"/>
         <v>2.2914213292021128</v>
       </c>
     </row>
-    <row r="142" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D142">
         <v>128</v>
       </c>
-      <c r="E142" s="7">
-        <f t="shared" si="1"/>
+      <c r="E142" s="6">
+        <f t="shared" si="4"/>
         <v>8.8199051570902725E-3</v>
       </c>
       <c r="F142" t="s">
@@ -4300,16 +4300,16 @@
         <v>154</v>
       </c>
       <c r="I142">
-        <f>255*E142</f>
+        <f t="shared" ref="I142:I149" si="6">255*E142</f>
         <v>2.2490758150580197</v>
       </c>
     </row>
-    <row r="143" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D143">
         <v>129</v>
       </c>
-      <c r="E143" s="7">
-        <f t="shared" ref="E143:E180" si="2">1/(((D143/100*3)+1)^3)</f>
+      <c r="E143" s="6">
+        <f t="shared" ref="E143:E149" si="7">1/(((D143/100*3)+1)^3)</f>
         <v>8.657910984779105E-3</v>
       </c>
       <c r="F143" t="s">
@@ -4319,16 +4319,16 @@
         <v>154</v>
       </c>
       <c r="I143">
-        <f>255*E143</f>
+        <f t="shared" si="6"/>
         <v>2.2077673011186718</v>
       </c>
     </row>
-    <row r="144" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D144">
         <v>130</v>
       </c>
-      <c r="E144" s="7">
-        <f t="shared" si="2"/>
+      <c r="E144" s="6">
+        <f t="shared" si="7"/>
         <v>8.4998597523140845E-3</v>
       </c>
       <c r="F144" t="s">
@@ -4338,16 +4338,16 @@
         <v>154</v>
       </c>
       <c r="I144">
-        <f>255*E144</f>
+        <f t="shared" si="6"/>
         <v>2.1674642368400914</v>
       </c>
     </row>
-    <row r="145" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D145">
         <v>131</v>
       </c>
-      <c r="E145" s="7">
-        <f t="shared" si="2"/>
+      <c r="E145" s="6">
+        <f t="shared" si="7"/>
         <v>8.3456322219919495E-3</v>
       </c>
       <c r="F145" t="s">
@@ -4357,16 +4357,16 @@
         <v>154</v>
       </c>
       <c r="I145">
-        <f>255*E145</f>
+        <f t="shared" si="6"/>
         <v>2.1281362166079472</v>
       </c>
     </row>
-    <row r="146" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D146">
         <v>132</v>
       </c>
-      <c r="E146" s="7">
-        <f t="shared" si="2"/>
+      <c r="E146" s="6">
+        <f t="shared" si="7"/>
         <v>8.1951134570843534E-3</v>
       </c>
       <c r="F146" t="s">
@@ -4376,16 +4376,16 @@
         <v>154</v>
       </c>
       <c r="I146">
-        <f>255*E146</f>
+        <f t="shared" si="6"/>
         <v>2.0897539315565101</v>
       </c>
     </row>
-    <row r="147" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D147">
         <v>133</v>
       </c>
-      <c r="E147" s="7">
-        <f t="shared" si="2"/>
+      <c r="E147" s="6">
+        <f t="shared" si="7"/>
         <v>8.0481926419253905E-3</v>
       </c>
       <c r="F147" t="s">
@@ -4395,16 +4395,16 @@
         <v>154</v>
       </c>
       <c r="I147">
-        <f>255*E147</f>
+        <f t="shared" si="6"/>
         <v>2.0522891236909744</v>
       </c>
     </row>
-    <row r="148" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D148">
         <v>134</v>
       </c>
-      <c r="E148" s="7">
-        <f t="shared" si="2"/>
+      <c r="E148" s="6">
+        <f t="shared" si="7"/>
         <v>7.9047629105488786E-3</v>
       </c>
       <c r="F148" t="s">
@@ -4414,16 +4414,16 @@
         <v>154</v>
       </c>
       <c r="I148">
-        <f>255*E148</f>
+        <f t="shared" si="6"/>
         <v>2.015714542189964</v>
       </c>
     </row>
-    <row r="149" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D149">
         <v>135</v>
       </c>
-      <c r="E149" s="7">
-        <f t="shared" si="2"/>
+      <c r="E149" s="6">
+        <f t="shared" si="7"/>
         <v>7.7647211834211529E-3</v>
       </c>
       <c r="F149" t="s">
@@ -4433,102 +4433,102 @@
         <v>154</v>
       </c>
       <c r="I149">
-        <f>255*E149</f>
+        <f t="shared" si="6"/>
         <v>1.980003901772394</v>
       </c>
     </row>
-    <row r="150" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E150" s="7"/>
-    </row>
-    <row r="151" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E151" s="7"/>
-    </row>
-    <row r="152" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E152" s="7"/>
-    </row>
-    <row r="153" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E153" s="7"/>
-    </row>
-    <row r="154" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E154" s="7"/>
-    </row>
-    <row r="155" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E155" s="7"/>
-    </row>
-    <row r="156" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E156" s="7"/>
-    </row>
-    <row r="157" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E157" s="7"/>
-    </row>
-    <row r="158" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E158" s="7"/>
-    </row>
-    <row r="159" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E159" s="7"/>
-    </row>
-    <row r="160" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="E160" s="7"/>
-    </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E161" s="7"/>
-    </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E162" s="7"/>
-    </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E163" s="7"/>
-    </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E164" s="7"/>
-    </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E165" s="7"/>
-    </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E166" s="7"/>
-    </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E167" s="7"/>
-    </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E168" s="7"/>
-    </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E169" s="7"/>
-    </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E170" s="7"/>
-    </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E171" s="7"/>
-    </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E172" s="7"/>
-    </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E173" s="7"/>
-    </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E174" s="7"/>
-    </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E175" s="7"/>
-    </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E176" s="7"/>
-    </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E177" s="7"/>
-    </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E178" s="7"/>
-    </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E179" s="7"/>
-    </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E180" s="7"/>
+    <row r="150" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E150" s="6"/>
+    </row>
+    <row r="151" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E151" s="6"/>
+    </row>
+    <row r="152" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E152" s="6"/>
+    </row>
+    <row r="153" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E153" s="6"/>
+    </row>
+    <row r="154" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E154" s="6"/>
+    </row>
+    <row r="155" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E155" s="6"/>
+    </row>
+    <row r="156" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E156" s="6"/>
+    </row>
+    <row r="157" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E157" s="6"/>
+    </row>
+    <row r="158" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E158" s="6"/>
+    </row>
+    <row r="159" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E159" s="6"/>
+    </row>
+    <row r="160" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E160" s="6"/>
+    </row>
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E161" s="6"/>
+    </row>
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E162" s="6"/>
+    </row>
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E163" s="6"/>
+    </row>
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E164" s="6"/>
+    </row>
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E165" s="6"/>
+    </row>
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E166" s="6"/>
+    </row>
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E167" s="6"/>
+    </row>
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E168" s="6"/>
+    </row>
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E169" s="6"/>
+    </row>
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E170" s="6"/>
+    </row>
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E171" s="6"/>
+    </row>
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E172" s="6"/>
+    </row>
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E173" s="6"/>
+    </row>
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E174" s="6"/>
+    </row>
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E175" s="6"/>
+    </row>
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E176" s="6"/>
+    </row>
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E177" s="6"/>
+    </row>
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E178" s="6"/>
+    </row>
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E179" s="6"/>
+    </row>
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E180" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4540,19 +4540,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F94E3F-4D34-4266-AA2E-47BA9E73B523}">
   <dimension ref="C5:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>136</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>53</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>53</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>53</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>53</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>53</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>53</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>53</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>53</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>53</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>53</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>53</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>53</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>53</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>53</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>53</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>53</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>53</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>53</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>85</v>
       </c>
@@ -4854,27 +4854,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>53</v>
       </c>
       <c r="D32" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>53</v>
       </c>
       <c r="D33" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>53</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>53</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>53</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>53</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>53</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>53</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>53</v>
       </c>
@@ -4984,7 +4984,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>53</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>53</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>53</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>53</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>53</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>53</v>
       </c>
@@ -5082,16 +5082,16 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>3</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -5107,13 +5107,13 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E9">
         <f>SUM(E7:E8)</f>
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>0</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>1</v>
       </c>
@@ -5129,24 +5129,24 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E15">
         <f>SUM(E13:E14)</f>
         <v>1.2999999999999998</v>
       </c>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>1.2</v>
       </c>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20">
         <f>0.6-0.35</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D21">
         <f>D20/2</f>
         <v>0.125</v>
@@ -5167,7 +5167,7 @@
         <v>168000000</v>
       </c>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D22">
         <f>D21+0.35</f>
         <v>0.47499999999999998</v>
@@ -5189,7 +5189,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
       <c r="L23" s="3">
         <f>N21/I22</f>
         <v>50.4</v>
@@ -5202,7 +5202,7 @@
         <v>3360000</v>
       </c>
     </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>8</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>2.976190476190476E-7</v>
       </c>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>10</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>7.1999999999999997E-6</v>
       </c>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>11</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>9</v>
       </c>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>12</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>14</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>15</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
         <v>17</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
         <v>18</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>5050</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>16</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
         <v>19</v>
       </c>
@@ -5322,23 +5322,23 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.26953125" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>32</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>33</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>35</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>0.1087646484375</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>37</v>
       </c>
@@ -5405,12 +5405,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>0.135955810546875</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>40</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>43</v>
       </c>
@@ -5443,12 +5443,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>42</v>
       </c>
@@ -5457,12 +5457,12 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>45</v>
       </c>
@@ -5484,9 +5484,9 @@
       <selection activeCell="T9" sqref="S9:T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>11</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>11</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>11</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>11</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>8</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>8</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>2</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>2</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12">
         <f>SUM(C3:C10)</f>
         <v>64</v>

</xml_diff>

<commit_message>
OLED Driver Change screen dimensions
</commit_message>
<xml_diff>
--- a/documentation/Pendulum General Notes.xlsx
+++ b/documentation/Pendulum General Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Github_Repos\Furuta-Pendulum\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A279326-1E3B-4472-B59B-4C7A49709E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EDD9E0-1688-4C6A-B9CD-56660F65BD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="4020" windowWidth="24540" windowHeight="13605" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NXP15XH103F03RC " sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="156">
   <si>
     <t>logic 1 high</t>
   </si>
@@ -331,9 +331,6 @@
     <t>USB_DP__LED_DO</t>
   </si>
   <si>
-    <t>soft button</t>
-  </si>
-  <si>
     <t>PA11</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
     <t>GPIO3</t>
   </si>
   <si>
-    <t>timing/spare</t>
-  </si>
-  <si>
     <t>PA1</t>
   </si>
   <si>
@@ -506,6 +500,15 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>soft button/timing</t>
+  </si>
+  <si>
+    <t>P/N: NXP15XH103F03RC , repurpose as SSD1357 nRST</t>
+  </si>
+  <si>
+    <t>dedicated boot0 pin :(</t>
   </si>
 </sst>
 </file>
@@ -1073,25 +1076,25 @@
   <sheetData>
     <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -1099,7 +1102,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C11">
         <f>2^C10</f>
@@ -1108,7 +1111,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C12">
         <v>3.3</v>
@@ -1116,7 +1119,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C13">
         <v>3300</v>
@@ -1129,22 +1132,22 @@
     </row>
     <row r="24" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F24">
         <v>10000</v>
       </c>
       <c r="G24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="5:15" x14ac:dyDescent="0.25">
@@ -1257,7 +1260,7 @@
         <v>422.82151095532726</v>
       </c>
       <c r="O29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="5:15" x14ac:dyDescent="0.25">
@@ -1304,7 +1307,7 @@
         <v>873.79138016950094</v>
       </c>
       <c r="O31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="5:15" x14ac:dyDescent="0.25">
@@ -1850,7 +1853,7 @@
   <sheetData>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
@@ -1862,10 +1865,10 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I14">
         <f t="shared" ref="I14:I45" si="0">255*E14</f>
@@ -1881,10 +1884,10 @@
         <v>0.91514165935315961</v>
       </c>
       <c r="F15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
@@ -1900,10 +1903,10 @@
         <v>0.8396192830323016</v>
       </c>
       <c r="F16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
@@ -1919,10 +1922,10 @@
         <v>0.77218348006106419</v>
       </c>
       <c r="F17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
@@ -1938,10 +1941,10 @@
         <v>0.71178024781341087</v>
       </c>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
@@ -1957,10 +1960,10 @@
         <v>0.65751623243198831</v>
       </c>
       <c r="F19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
@@ -1976,10 +1979,10 @@
         <v>0.6086308726792905</v>
       </c>
       <c r="F20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
@@ -1995,10 +1998,10 @@
         <v>0.56447393005377744</v>
       </c>
       <c r="F21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
@@ -2014,10 +2017,10 @@
         <v>0.52448726125339862</v>
       </c>
       <c r="F22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
@@ -2033,10 +2036,10 @@
         <v>0.48818995275785831</v>
       </c>
       <c r="F23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
@@ -2052,10 +2055,10 @@
         <v>0.45516613563950831</v>
       </c>
       <c r="F24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
@@ -2071,10 +2074,10 @@
         <v>0.42505494897852919</v>
       </c>
       <c r="F25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
@@ -2090,10 +2093,10 @@
         <v>0.3975422348870345</v>
       </c>
       <c r="F26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
@@ -2109,10 +2112,10 @@
         <v>0.3723536361635808</v>
       </c>
       <c r="F27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
@@ -2128,10 +2131,10 @@
         <v>0.34924883560438214</v>
       </c>
       <c r="F28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
@@ -2147,10 +2150,10 @@
         <v>0.32801672885317151</v>
       </c>
       <c r="F29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
@@ -2166,10 +2169,10 @@
         <v>0.30847136398633845</v>
       </c>
       <c r="F30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
@@ -2185,10 +2188,10 @@
         <v>0.29044851349903034</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
@@ -2204,10 +2207,10 @@
         <v>0.27380277000786363</v>
       </c>
       <c r="F32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
@@ -2223,10 +2226,10 @@
         <v>0.25840507734968382</v>
       </c>
       <c r="F33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
@@ -2242,10 +2245,10 @@
         <v>0.24414062499999994</v>
       </c>
       <c r="F34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
@@ -2261,10 +2264,10 @@
         <v>0.23090704675198068</v>
       </c>
       <c r="F35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
@@ -2280,10 +2283,10 @@
         <v>0.2186128750741097</v>
       </c>
       <c r="F36" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
@@ -2299,10 +2302,10 @@
         <v>0.20717621103300343</v>
       </c>
       <c r="F37" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G37" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
@@ -2318,10 +2321,10 @@
         <v>0.19652357654043043</v>
       </c>
       <c r="F38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
@@ -2337,10 +2340,10 @@
         <v>0.18658892128279883</v>
       </c>
       <c r="F39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G39" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
@@ -2356,10 +2359,10 @@
         <v>0.17731276127035372</v>
       </c>
       <c r="F40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
@@ -2375,10 +2378,10 @@
         <v>0.16864142970156706</v>
       </c>
       <c r="F41" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
@@ -2394,10 +2397,10 @@
         <v>0.16052642393359084</v>
       </c>
       <c r="F42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
@@ -2413,10 +2416,10 @@
         <v>0.15292383490770972</v>
       </c>
       <c r="F43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G43" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
@@ -2432,10 +2435,10 @@
         <v>0.14579384749963553</v>
       </c>
       <c r="F44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
@@ -2451,10 +2454,10 @@
         <v>0.13910030202848581</v>
       </c>
       <c r="F45" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G45" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
@@ -2470,10 +2473,10 @@
         <v>0.13281030862990761</v>
       </c>
       <c r="F46" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G46" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I46">
         <f t="shared" ref="I46:I77" si="2">255*E46</f>
@@ -2489,10 +2492,10 @@
         <v>0.12689390743013315</v>
       </c>
       <c r="F47" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G47" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I47">
         <f t="shared" si="2"/>
@@ -2508,10 +2511,10 @@
         <v>0.12132376849095557</v>
       </c>
       <c r="F48" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G48" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I48">
         <f t="shared" si="2"/>
@@ -2527,10 +2530,10 @@
         <v>0.11607492636496861</v>
       </c>
       <c r="F49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G49" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I49">
         <f t="shared" si="2"/>
@@ -2546,10 +2549,10 @@
         <v>0.11112454483386436</v>
       </c>
       <c r="F50" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I50">
         <f t="shared" si="2"/>
@@ -2565,10 +2568,10 @@
         <v>0.10645170802297783</v>
       </c>
       <c r="F51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I51">
         <f t="shared" si="2"/>
@@ -2584,10 +2587,10 @@
         <v>0.10203723461135648</v>
       </c>
       <c r="F52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G52" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I52">
         <f t="shared" si="2"/>
@@ -2603,10 +2606,10 @@
         <v>9.7863512303841146E-2</v>
       </c>
       <c r="F53" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I53">
         <f t="shared" si="2"/>
@@ -2622,10 +2625,10 @@
         <v>9.3914350112697192E-2</v>
       </c>
       <c r="F54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I54">
         <f t="shared" si="2"/>
@@ -2641,10 +2644,10 @@
         <v>9.0174846321772528E-2</v>
       </c>
       <c r="F55" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I55">
         <f t="shared" si="2"/>
@@ -2660,10 +2663,10 @@
         <v>8.6631270284711973E-2</v>
       </c>
       <c r="F56" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G56" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I56">
         <f t="shared" si="2"/>
@@ -2679,10 +2682,10 @@
         <v>8.3270956447707614E-2</v>
       </c>
       <c r="F57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G57" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I57">
         <f t="shared" si="2"/>
@@ -2698,10 +2701,10 @@
         <v>8.0082209192668799E-2</v>
       </c>
       <c r="F58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G58" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I58">
         <f t="shared" si="2"/>
@@ -2717,10 +2720,10 @@
         <v>7.7054217273629141E-2</v>
       </c>
       <c r="F59" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G59" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I59">
         <f t="shared" si="2"/>
@@ -2736,10 +2739,10 @@
         <v>7.4176976771924794E-2</v>
       </c>
       <c r="F60" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G60" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I60">
         <f t="shared" si="2"/>
@@ -2755,10 +2758,10 @@
         <v>7.1441221627743925E-2</v>
       </c>
       <c r="F61" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G61" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I61">
         <f t="shared" si="2"/>
@@ -2774,10 +2777,10 @@
         <v>6.8838360920077016E-2</v>
       </c>
       <c r="F62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G62" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I62">
         <f t="shared" si="2"/>
@@ -2793,10 +2796,10 @@
         <v>6.6360422166424932E-2</v>
       </c>
       <c r="F63" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I63">
         <f t="shared" si="2"/>
@@ -2812,10 +2815,10 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="F64" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G64" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I64">
         <f t="shared" si="2"/>
@@ -2831,10 +2834,10 @@
         <v>6.175020965739933E-2</v>
       </c>
       <c r="F65" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I65">
         <f t="shared" si="2"/>
@@ -2850,10 +2853,10 @@
         <v>5.9604644775390618E-2</v>
       </c>
       <c r="F66" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G66" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I66">
         <f t="shared" si="2"/>
@@ -2869,10 +2872,10 @@
         <v>5.7557339052844506E-2</v>
       </c>
       <c r="F67" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G67" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I67">
         <f t="shared" si="2"/>
@@ -2888,10 +2891,10 @@
         <v>5.5602731384094314E-2</v>
       </c>
       <c r="F68" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G68" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I68">
         <f t="shared" si="2"/>
@@ -2907,10 +2910,10 @@
         <v>5.3735634114067295E-2</v>
       </c>
       <c r="F69" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G69" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I69">
         <f t="shared" si="2"/>
@@ -2926,10 +2929,10 @@
         <v>5.1951204104228238E-2</v>
       </c>
       <c r="F70" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G70" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I70">
         <f t="shared" si="2"/>
@@ -2945,10 +2948,10 @@
         <v>5.0244916332416546E-2</v>
       </c>
       <c r="F71" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G71" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I71">
         <f t="shared" si="2"/>
@@ -2964,10 +2967,10 @@
         <v>4.8612539779641313E-2</v>
       </c>
       <c r="F72" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G72" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I72">
         <f t="shared" si="2"/>
@@ -2983,10 +2986,10 @@
         <v>4.7050115383350459E-2</v>
       </c>
       <c r="F73" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G73" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I73">
         <f t="shared" si="2"/>
@@ -3002,10 +3005,10 @@
         <v>4.555393586005832E-2</v>
       </c>
       <c r="F74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G74" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I74">
         <f t="shared" si="2"/>
@@ -3021,10 +3024,10 @@
         <v>4.4120527220887253E-2</v>
       </c>
       <c r="F75" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G75" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I75">
         <f t="shared" si="2"/>
@@ -3040,10 +3043,10 @@
         <v>4.2746631821892235E-2</v>
       </c>
       <c r="F76" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G76" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I76">
         <f t="shared" si="2"/>
@@ -3059,10 +3062,10 @@
         <v>4.1429192807278969E-2</v>
       </c>
       <c r="F77" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G77" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I77">
         <f t="shared" si="2"/>
@@ -3078,10 +3081,10 @@
         <v>4.016533981805423E-2</v>
       </c>
       <c r="F78" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G78" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I78">
         <f t="shared" ref="I78:I109" si="3">255*E78</f>
@@ -3097,10 +3100,10 @@
         <v>3.895237585147459E-2</v>
       </c>
       <c r="F79" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G79" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I79">
         <f t="shared" si="3"/>
@@ -3116,10 +3119,10 @@
         <v>3.7787765168084519E-2</v>
       </c>
       <c r="F80" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G80" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I80">
         <f t="shared" si="3"/>
@@ -3135,10 +3138,10 @@
         <v>3.6669122153316448E-2</v>
       </c>
       <c r="F81" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G81" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I81">
         <f t="shared" si="3"/>
@@ -3154,10 +3157,10 @@
         <v>3.5594201049715703E-2</v>
       </c>
       <c r="F82" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G82" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I82">
         <f t="shared" si="3"/>
@@ -3173,10 +3176,10 @@
         <v>3.4560886483973451E-2</v>
       </c>
       <c r="F83" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G83" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I83">
         <f t="shared" si="3"/>
@@ -3192,10 +3195,10 @@
         <v>3.3567184720217524E-2</v>
       </c>
       <c r="F84" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I84">
         <f t="shared" si="3"/>
@@ -3211,10 +3214,10 @@
         <v>3.2611215577516749E-2</v>
       </c>
       <c r="F85" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G85" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I85">
         <f t="shared" si="3"/>
@@ -3230,10 +3233,10 @@
         <v>3.1691204955388914E-2</v>
       </c>
       <c r="F86" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G86" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I86">
         <f t="shared" si="3"/>
@@ -3249,10 +3252,10 @@
         <v>3.080547791633842E-2</v>
       </c>
       <c r="F87" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G87" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I87">
         <f t="shared" si="3"/>
@@ -3268,10 +3271,10 @@
         <v>2.9952452279153993E-2</v>
       </c>
       <c r="F88" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G88" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I88">
         <f t="shared" si="3"/>
@@ -3287,10 +3290,10 @@
         <v>2.9130632680928539E-2</v>
       </c>
       <c r="F89" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G89" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I89">
         <f t="shared" si="3"/>
@@ -3306,10 +3309,10 @@
         <v>2.8338605069572406E-2</v>
       </c>
       <c r="F90" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G90" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I90">
         <f t="shared" si="3"/>
@@ -3325,10 +3328,10 @@
         <v>2.7575031592024315E-2</v>
       </c>
       <c r="F91" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G91" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I91">
         <f t="shared" si="3"/>
@@ -3344,10 +3347,10 @@
         <v>2.6838645846461905E-2</v>
       </c>
       <c r="F92" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G92" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I92">
         <f t="shared" si="3"/>
@@ -3363,10 +3366,10 @@
         <v>2.6128248469609691E-2</v>
       </c>
       <c r="F93" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G93" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I93">
         <f t="shared" si="3"/>
@@ -3382,10 +3385,10 @@
         <v>2.5442703032770197E-2</v>
       </c>
       <c r="F94" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G94" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I94">
         <f t="shared" si="3"/>
@@ -3401,10 +3404,10 @@
         <v>2.4780932222490046E-2</v>
       </c>
       <c r="F95" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G95" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I95">
         <f t="shared" si="3"/>
@@ -3420,10 +3423,10 @@
         <v>2.414191428384363E-2</v>
       </c>
       <c r="F96" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G96" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I96">
         <f t="shared" si="3"/>
@@ -3439,10 +3442,10 @@
         <v>2.3524679706192753E-2</v>
       </c>
       <c r="F97" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G97" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I97">
         <f t="shared" si="3"/>
@@ -3458,10 +3461,10 @@
         <v>2.292830813298272E-2</v>
       </c>
       <c r="F98" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G98" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I98">
         <f t="shared" si="3"/>
@@ -3477,10 +3480,10 @@
         <v>2.2351925478680458E-2</v>
       </c>
       <c r="F99" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G99" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I99">
         <f t="shared" si="3"/>
@@ -3496,10 +3499,10 @@
         <v>2.1794701237363653E-2</v>
       </c>
       <c r="F100" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G100" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I100">
         <f t="shared" si="3"/>
@@ -3515,10 +3518,10 @@
         <v>2.1255845968746981E-2</v>
       </c>
       <c r="F101" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G101" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I101">
         <f t="shared" si="3"/>
@@ -3534,10 +3537,10 @@
         <v>2.0734608948592765E-2</v>
       </c>
       <c r="F102" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G102" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I102">
         <f t="shared" si="3"/>
@@ -3553,10 +3556,10 @@
         <v>2.0230275971511971E-2</v>
       </c>
       <c r="F103" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G103" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I103">
         <f t="shared" si="3"/>
@@ -3572,10 +3575,10 @@
         <v>1.9742167295125658E-2</v>
       </c>
       <c r="F104" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G104" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I104">
         <f t="shared" si="3"/>
@@ -3591,10 +3594,10 @@
         <v>1.9269635715437352E-2</v>
       </c>
       <c r="F105" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G105" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I105">
         <f t="shared" si="3"/>
@@ -3610,10 +3613,10 @@
         <v>1.8812064764069613E-2</v>
       </c>
       <c r="F106" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G106" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I106">
         <f t="shared" si="3"/>
@@ -3629,10 +3632,10 @@
         <v>1.8368867018752538E-2</v>
       </c>
       <c r="F107" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G107" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I107">
         <f t="shared" si="3"/>
@@ -3648,10 +3651,10 @@
         <v>1.7939482519122411E-2</v>
       </c>
       <c r="F108" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G108" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I108">
         <f t="shared" si="3"/>
@@ -3667,10 +3670,10 @@
         <v>1.7523377280503277E-2</v>
       </c>
       <c r="F109" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G109" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I109">
         <f t="shared" si="3"/>
@@ -3686,10 +3689,10 @@
         <v>1.7120041898905744E-2</v>
       </c>
       <c r="F110" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G110" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I110">
         <f t="shared" ref="I110:I141" si="5">255*E110</f>
@@ -3705,10 +3708,10 @@
         <v>1.6728990240992978E-2</v>
       </c>
       <c r="F111" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G111" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I111">
         <f t="shared" si="5"/>
@@ -3724,10 +3727,10 @@
         <v>1.634975821323564E-2</v>
       </c>
       <c r="F112" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G112" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I112">
         <f t="shared" si="5"/>
@@ -3743,10 +3746,10 @@
         <v>1.5981902604911086E-2</v>
       </c>
       <c r="F113" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G113" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I113">
         <f t="shared" si="5"/>
@@ -3762,10 +3765,10 @@
         <v>1.5625E-2</v>
       </c>
       <c r="F114" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G114" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I114">
         <f t="shared" si="5"/>
@@ -3781,10 +3784,10 @@
         <v>1.5278645753398956E-2</v>
       </c>
       <c r="F115" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G115" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I115">
         <f t="shared" si="5"/>
@@ -3800,10 +3803,10 @@
         <v>1.4942453027203508E-2</v>
       </c>
       <c r="F116" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G116" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I116">
         <f t="shared" si="5"/>
@@ -3819,10 +3822,10 @@
         <v>1.461605188312555E-2</v>
       </c>
       <c r="F117" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G117" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I117">
         <f t="shared" si="5"/>
@@ -3838,10 +3841,10 @@
         <v>1.4299088427393119E-2</v>
       </c>
       <c r="F118" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G118" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I118">
         <f t="shared" si="5"/>
@@ -3857,10 +3860,10 @@
         <v>1.3991224004743022E-2</v>
       </c>
       <c r="F119" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G119" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I119">
         <f t="shared" si="5"/>
@@ -3876,10 +3879,10 @@
         <v>1.3692134438357957E-2</v>
       </c>
       <c r="F120" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G120" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I120">
         <f t="shared" si="5"/>
@@ -3895,10 +3898,10 @@
         <v>1.3401509312822735E-2</v>
       </c>
       <c r="F121" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G121" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I121">
         <f t="shared" si="5"/>
@@ -3914,10 +3917,10 @@
         <v>1.3119051297379712E-2</v>
       </c>
       <c r="F122" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G122" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I122">
         <f t="shared" si="5"/>
@@ -3933,10 +3936,10 @@
         <v>1.284447550695314E-2</v>
       </c>
       <c r="F123" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G123" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I123">
         <f t="shared" si="5"/>
@@ -3952,10 +3955,10 @@
         <v>1.2577508898587541E-2</v>
       </c>
       <c r="F124" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G124" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I124">
         <f t="shared" si="5"/>
@@ -3971,10 +3974,10 @@
         <v>1.2317889701107268E-2</v>
       </c>
       <c r="F125" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G125" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I125">
         <f t="shared" si="5"/>
@@ -3990,10 +3993,10 @@
         <v>1.2065366875954128E-2</v>
       </c>
       <c r="F126" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G126" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I126">
         <f t="shared" si="5"/>
@@ -4009,10 +4012,10 @@
         <v>1.1819699607298758E-2</v>
       </c>
       <c r="F127" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G127" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I127">
         <f t="shared" si="5"/>
@@ -4028,10 +4031,10 @@
         <v>1.1580656819649614E-2</v>
       </c>
       <c r="F128" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G128" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I128">
         <f t="shared" si="5"/>
@@ -4047,10 +4050,10 @@
         <v>1.1348016721302643E-2</v>
       </c>
       <c r="F129" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G129" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I129">
         <f t="shared" si="5"/>
@@ -4066,10 +4069,10 @@
         <v>1.1121566372084552E-2</v>
       </c>
       <c r="F130" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G130" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I130">
         <f t="shared" si="5"/>
@@ -4085,10 +4088,10 @@
         <v>1.090110127394521E-2</v>
       </c>
       <c r="F131" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G131" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I131">
         <f t="shared" si="5"/>
@@ -4104,10 +4107,10 @@
         <v>1.0686424983049194E-2</v>
       </c>
       <c r="F132" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G132" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I132">
         <f t="shared" si="5"/>
@@ -4123,10 +4126,10 @@
         <v>1.04773487421047E-2</v>
       </c>
       <c r="F133" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G133" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I133">
         <f t="shared" si="5"/>
@@ -4142,10 +4145,10 @@
         <v>1.0273691131749817E-2</v>
       </c>
       <c r="F134" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G134" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I134">
         <f t="shared" si="5"/>
@@ -4161,10 +4164,10 @@
         <v>1.0075277739891936E-2</v>
       </c>
       <c r="F135" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G135" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I135">
         <f t="shared" si="5"/>
@@ -4180,10 +4183,10 @@
         <v>9.8819408479669715E-3</v>
       </c>
       <c r="F136" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G136" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I136">
         <f t="shared" si="5"/>
@@ -4199,10 +4202,10 @@
         <v>9.693519133150464E-3</v>
       </c>
       <c r="F137" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G137" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I137">
         <f t="shared" si="5"/>
@@ -4218,10 +4221,10 @@
         <v>9.5098573856139141E-3</v>
       </c>
       <c r="F138" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G138" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I138">
         <f t="shared" si="5"/>
@@ -4237,10 +4240,10 @@
         <v>9.3308062399766727E-3</v>
       </c>
       <c r="F139" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G139" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I139">
         <f t="shared" si="5"/>
@@ -4256,10 +4259,10 @@
         <v>9.1562219201564259E-3</v>
       </c>
       <c r="F140" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G140" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I140">
         <f t="shared" si="5"/>
@@ -4275,10 +4278,10 @@
         <v>8.9859659968710304E-3</v>
       </c>
       <c r="F141" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G141" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I141">
         <f t="shared" si="5"/>
@@ -4294,10 +4297,10 @@
         <v>8.8199051570902725E-3</v>
       </c>
       <c r="F142" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G142" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I142">
         <f t="shared" ref="I142:I149" si="6">255*E142</f>
@@ -4313,10 +4316,10 @@
         <v>8.657910984779105E-3</v>
       </c>
       <c r="F143" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G143" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I143">
         <f t="shared" si="6"/>
@@ -4332,10 +4335,10 @@
         <v>8.4998597523140845E-3</v>
       </c>
       <c r="F144" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G144" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I144">
         <f t="shared" si="6"/>
@@ -4351,10 +4354,10 @@
         <v>8.3456322219919495E-3</v>
       </c>
       <c r="F145" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G145" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I145">
         <f t="shared" si="6"/>
@@ -4370,10 +4373,10 @@
         <v>8.1951134570843534E-3</v>
       </c>
       <c r="F146" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G146" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I146">
         <f t="shared" si="6"/>
@@ -4389,10 +4392,10 @@
         <v>8.0481926419253905E-3</v>
       </c>
       <c r="F147" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G147" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I147">
         <f t="shared" si="6"/>
@@ -4408,10 +4411,10 @@
         <v>7.9047629105488786E-3</v>
       </c>
       <c r="F148" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G148" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I148">
         <f t="shared" si="6"/>
@@ -4427,10 +4430,10 @@
         <v>7.7647211834211529E-3</v>
       </c>
       <c r="F149" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G149" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I149">
         <f t="shared" si="6"/>
@@ -4540,30 +4543,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F94E3F-4D34-4266-AA2E-47BA9E73B523}">
   <dimension ref="C5:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
@@ -4571,13 +4574,13 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G6" t="s">
         <v>64</v>
@@ -4588,13 +4591,13 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="G7" t="s">
         <v>64</v>
@@ -4605,19 +4608,19 @@
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8" t="s">
         <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
@@ -4625,19 +4628,19 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G9" t="s">
         <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
@@ -4645,10 +4648,10 @@
         <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G11" t="s">
         <v>64</v>
@@ -4659,10 +4662,10 @@
         <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G12" t="s">
         <v>64</v>
@@ -4673,10 +4676,10 @@
         <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G13" t="s">
         <v>64</v>
@@ -4687,10 +4690,10 @@
         <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G14" t="s">
         <v>64</v>
@@ -4701,13 +4704,13 @@
         <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G15" t="s">
         <v>64</v>
@@ -4718,10 +4721,10 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" t="s">
         <v>64</v>
@@ -4732,10 +4735,10 @@
         <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G18" t="s">
         <v>64</v>
@@ -4746,10 +4749,10 @@
         <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G20" t="s">
         <v>64</v>
@@ -4760,10 +4763,10 @@
         <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G21" t="s">
         <v>64</v>
@@ -4774,10 +4777,10 @@
         <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" t="s">
@@ -4789,13 +4792,13 @@
         <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
@@ -4851,7 +4854,7 @@
         <v>85</v>
       </c>
       <c r="F30" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
@@ -5048,7 +5051,7 @@
         <v>55</v>
       </c>
       <c r="F47" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fucked everything up its my repo i can name commits whatever i wants
</commit_message>
<xml_diff>
--- a/documentation/Pendulum General Notes.xlsx
+++ b/documentation/Pendulum General Notes.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Github_Repos\Furuta-Pendulum\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ross\Documents\GitHub\Furuta-Pendulum\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EDD9E0-1688-4C6A-B9CD-56660F65BD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CC8592-6EC5-4F88-A38B-C405FA92ABE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="4020" windowWidth="24540" windowHeight="13605" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4670" yWindow="3860" windowWidth="19200" windowHeight="11260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NXP15XH103F03RC " sheetId="5" r:id="rId1"/>
-    <sheet name="LED Q shaped Pulse LUT" sheetId="6" r:id="rId2"/>
-    <sheet name="Pinout" sheetId="4" r:id="rId3"/>
-    <sheet name="LED Driver" sheetId="1" r:id="rId4"/>
-    <sheet name="Shunt Value Calculation" sheetId="3" r:id="rId5"/>
-    <sheet name="CAN Notes" sheetId="2" r:id="rId6"/>
+    <sheet name="PLL config" sheetId="7" r:id="rId2"/>
+    <sheet name="LED Q shaped Pulse LUT" sheetId="6" r:id="rId3"/>
+    <sheet name="Pinout" sheetId="4" r:id="rId4"/>
+    <sheet name="LED Driver" sheetId="1" r:id="rId5"/>
+    <sheet name="Shunt Value Calculation" sheetId="3" r:id="rId6"/>
+    <sheet name="CAN Notes" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="168">
   <si>
     <t>logic 1 high</t>
   </si>
@@ -509,6 +510,42 @@
   </si>
   <si>
     <t>dedicated boot0 pin :(</t>
+  </si>
+  <si>
+    <t>8 to 127</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>1 to 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m </t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>2, 4, 6, 8</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R, Q</t>
+  </si>
+  <si>
+    <t>7, 17, 2-31</t>
   </si>
 </sst>
 </file>
@@ -700,6 +737,50 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6658904" cy="1667108"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9C28372-B021-4008-9600-12ADE1649D44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3841750" y="1454150"/>
+          <a:ext cx="6658904" cy="1667108"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -747,7 +828,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1065,16 +1146,16 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>149</v>
       </c>
@@ -1082,17 +1163,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>145</v>
       </c>
@@ -1100,7 +1181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>144</v>
       </c>
@@ -1109,7 +1190,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>143</v>
       </c>
@@ -1117,7 +1198,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>142</v>
       </c>
@@ -1125,12 +1206,12 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:15" x14ac:dyDescent="0.35">
       <c r="H21">
         <v>274.14999999999998</v>
       </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E24" t="s">
         <v>141</v>
       </c>
@@ -1150,7 +1231,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E25">
         <v>3455</v>
       </c>
@@ -1172,7 +1253,7 @@
         <v>54.039423557411865</v>
       </c>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E26">
         <v>3455</v>
       </c>
@@ -1194,7 +1275,7 @@
         <v>97.82536621618496</v>
       </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E27">
         <v>3455</v>
       </c>
@@ -1216,7 +1297,7 @@
         <v>167.72873235490044</v>
       </c>
     </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E28">
         <v>3455</v>
       </c>
@@ -1238,7 +1319,7 @@
         <v>273.09089816363326</v>
       </c>
     </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E29">
         <v>3455</v>
       </c>
@@ -1263,7 +1344,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E30">
         <v>3455</v>
       </c>
@@ -1285,7 +1366,7 @@
         <v>622.93869172748441</v>
       </c>
     </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E31">
         <v>3455</v>
       </c>
@@ -1310,7 +1391,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:15" x14ac:dyDescent="0.35">
       <c r="E32">
         <v>3455</v>
       </c>
@@ -1332,7 +1413,7 @@
         <v>1168.1899374657055</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E33">
         <v>3455</v>
       </c>
@@ -1354,7 +1435,7 @@
         <v>1491.7416415985278</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E34">
         <v>3455</v>
       </c>
@@ -1376,7 +1457,7 @@
         <v>1825.7304907981015</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E35">
         <v>3455</v>
       </c>
@@ -1398,7 +1479,7 @@
         <v>2151.396943141714</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E36">
         <v>3455</v>
       </c>
@@ -1420,7 +1501,7 @@
         <v>2453.7008277400541</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E37">
         <v>3455</v>
       </c>
@@ -1442,7 +1523,7 @@
         <v>2723.2172426961902</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E38">
         <v>3455</v>
       </c>
@@ -1464,7 +1545,7 @@
         <v>2956.0577198229148</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E39">
         <v>3455</v>
       </c>
@@ -1486,7 +1567,7 @@
         <v>3152.5786257994127</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E40">
         <v>3455</v>
       </c>
@@ -1508,7 +1589,7 @@
         <v>3315.7626168202719</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E41">
         <v>3455</v>
       </c>
@@ -1530,7 +1611,7 @@
         <v>3449.8361873826639</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E42">
         <v>3455</v>
       </c>
@@ -1552,7 +1633,7 @@
         <v>3559.3192522629574</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E43">
         <v>3455</v>
       </c>
@@ -1574,7 +1655,7 @@
         <v>3648.4778466001449</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E44">
         <v>3455</v>
       </c>
@@ -1596,7 +1677,7 @@
         <v>3721.0689591442965</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E45">
         <v>3455</v>
       </c>
@@ -1618,7 +1699,7 @@
         <v>3780.2656325848657</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E46">
         <v>3455</v>
       </c>
@@ -1640,7 +1721,7 @@
         <v>3828.6787150076775</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E47">
         <v>3455</v>
       </c>
@@ -1662,7 +1743,7 @@
         <v>3868.4219508381043</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E48">
         <v>3455</v>
       </c>
@@ -1684,7 +1765,7 @@
         <v>3901.1901499119167</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E49">
         <v>3455</v>
       </c>
@@ -1706,127 +1787,127 @@
         <v>3928.3351114386833</v>
       </c>
     </row>
-    <row r="55" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F55">
         <v>-40</v>
       </c>
     </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F56">
         <v>-30</v>
       </c>
     </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F57">
         <v>-20</v>
       </c>
     </row>
-    <row r="58" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F58">
         <v>-10</v>
       </c>
     </row>
-    <row r="59" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F60">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F61">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F62">
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F63">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F64">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F65">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F66">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F67">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F68">
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F69">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F70">
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F71">
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F72">
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F73">
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F74">
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F75">
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F76">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F77">
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F78">
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F79">
         <v>200</v>
       </c>
@@ -1839,6 +1920,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0256D11-FC41-4AB2-818C-45B065599BCC}">
+  <dimension ref="B1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="11.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <f>C3*(D3/E3)</f>
+        <v>340</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>85</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>159</v>
+      </c>
+      <c r="J3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>157</v>
+      </c>
+      <c r="J4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <f>340/16</f>
+        <v>21.25</v>
+      </c>
+      <c r="C7">
+        <f>B7*8</f>
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0F148E-F223-466A-A7C9-AAB69A928868}">
   <dimension ref="C11:I180"/>
   <sheetViews>
@@ -1846,17 +2013,17 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D14">
         <v>0</v>
       </c>
@@ -1875,7 +2042,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D15">
         <v>1</v>
       </c>
@@ -1894,7 +2061,7 @@
         <v>233.36112313505569</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D16">
         <v>2</v>
       </c>
@@ -1913,7 +2080,7 @@
         <v>214.1029171732369</v>
       </c>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D17">
         <v>3</v>
       </c>
@@ -1932,7 +2099,7 @@
         <v>196.90678741557136</v>
       </c>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D18">
         <v>4</v>
       </c>
@@ -1951,7 +2118,7 @@
         <v>181.50396319241977</v>
       </c>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D19">
         <v>5</v>
       </c>
@@ -1970,7 +2137,7 @@
         <v>167.66663927015702</v>
       </c>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D20">
         <v>6</v>
       </c>
@@ -1989,7 +2156,7 @@
         <v>155.20087253321907</v>
       </c>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D21">
         <v>7</v>
       </c>
@@ -2008,7 +2175,7 @@
         <v>143.94085216371326</v>
       </c>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D22">
         <v>8</v>
       </c>
@@ -2027,7 +2194,7 @@
         <v>133.74425161961665</v>
       </c>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D23">
         <v>9</v>
       </c>
@@ -2046,7 +2213,7 @@
         <v>124.48843795325386</v>
       </c>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D24">
         <v>10</v>
       </c>
@@ -2065,7 +2232,7 @@
         <v>116.06736458807462</v>
       </c>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D25">
         <v>11</v>
       </c>
@@ -2084,7 +2251,7 @@
         <v>108.38901198952495</v>
       </c>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D26">
         <v>12</v>
       </c>
@@ -2103,7 +2270,7 @@
         <v>101.37326989619379</v>
       </c>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D27">
         <v>13</v>
       </c>
@@ -2122,7 +2289,7 @@
         <v>94.950177221713105</v>
       </c>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D28">
         <v>14</v>
       </c>
@@ -2141,7 +2308,7 @@
         <v>89.058453079117442</v>
       </c>
     </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D29">
         <v>15</v>
       </c>
@@ -2160,7 +2327,7 @@
         <v>83.644265857558736</v>
       </c>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D30">
         <v>16</v>
       </c>
@@ -2179,7 +2346,7 @@
         <v>78.660197816516302</v>
       </c>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D31">
         <v>17</v>
       </c>
@@ -2198,7 +2365,7 @@
         <v>74.064370942252737</v>
       </c>
     </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D32">
         <v>18</v>
       </c>
@@ -2217,7 +2384,7 @@
         <v>69.819706352005227</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D33">
         <v>19</v>
       </c>
@@ -2236,7 +2403,7 @@
         <v>65.89329472416938</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D34">
         <v>20</v>
       </c>
@@ -2255,7 +2422,7 @@
         <v>62.255859374999986</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D35">
         <v>21</v>
       </c>
@@ -2274,7 +2441,7 @@
         <v>58.881296921755073</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D36">
         <v>22</v>
       </c>
@@ -2293,7 +2460,7 @@
         <v>55.746283143897976</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D37">
         <v>23</v>
       </c>
@@ -2312,7 +2479,7 @@
         <v>52.829933813415877</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D38">
         <v>24</v>
       </c>
@@ -2331,7 +2498,7 @@
         <v>50.113512017809761</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D39">
         <v>25</v>
       </c>
@@ -2350,7 +2517,7 @@
         <v>47.580174927113703</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D40">
         <v>26</v>
       </c>
@@ -2369,7 +2536,7 @@
         <v>45.214754123940203</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D41">
         <v>27</v>
       </c>
@@ -2388,7 +2555,7 @@
         <v>43.003564573899602</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D42">
         <v>28</v>
       </c>
@@ -2407,7 +2574,7 @@
         <v>40.934238103065667</v>
       </c>
     </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D43">
         <v>29</v>
       </c>
@@ -2426,7 +2593,7 @@
         <v>38.995577901465978</v>
       </c>
     </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D44">
         <v>30</v>
       </c>
@@ -2445,7 +2612,7 @@
         <v>37.177431112407064</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D45">
         <v>31</v>
       </c>
@@ -2464,7 +2631,7 @@
         <v>35.470577017263878</v>
       </c>
     </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D46">
         <v>32</v>
       </c>
@@ -2483,7 +2650,7 @@
         <v>33.866628700626443</v>
       </c>
     </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D47">
         <v>33</v>
       </c>
@@ -2502,7 +2669,7 @@
         <v>32.357946394683957</v>
       </c>
     </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D48">
         <v>34</v>
       </c>
@@ -2521,7 +2688,7 @@
         <v>30.937560965193668</v>
       </c>
     </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D49">
         <v>35</v>
       </c>
@@ -2540,7 +2707,7 @@
         <v>29.599106223066993</v>
       </c>
     </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D50">
         <v>36</v>
       </c>
@@ -2559,7 +2726,7 @@
         <v>28.336758932635412</v>
       </c>
     </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D51">
         <v>37</v>
       </c>
@@ -2578,7 +2745,7 @@
         <v>27.145185545859349</v>
       </c>
     </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D52">
         <v>38</v>
       </c>
@@ -2597,7 +2764,7 @@
         <v>26.019494825895904</v>
       </c>
     </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D53">
         <v>39</v>
       </c>
@@ -2616,7 +2783,7 @@
         <v>24.955195637479491</v>
       </c>
     </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D54">
         <v>40</v>
       </c>
@@ -2635,7 +2802,7 @@
         <v>23.948159278737783</v>
       </c>
     </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D55">
         <v>41</v>
       </c>
@@ -2654,7 +2821,7 @@
         <v>22.994585812051994</v>
       </c>
     </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D56">
         <v>42</v>
       </c>
@@ -2673,7 +2840,7 @@
         <v>22.090973922601552</v>
       </c>
     </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D57">
         <v>43</v>
       </c>
@@ -2692,7 +2859,7 @@
         <v>21.23409389416544</v>
       </c>
     </row>
-    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D58">
         <v>44</v>
       </c>
@@ -2711,7 +2878,7 @@
         <v>20.420963344130545</v>
       </c>
     </row>
-    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D59">
         <v>45</v>
       </c>
@@ -2730,7 +2897,7 @@
         <v>19.64882540477543</v>
       </c>
     </row>
-    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D60">
         <v>46</v>
       </c>
@@ -2749,7 +2916,7 @@
         <v>18.915129076840824</v>
       </c>
     </row>
-    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D61">
         <v>47</v>
       </c>
@@ -2768,7 +2935,7 @@
         <v>18.217511515074701</v>
       </c>
     </row>
-    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D62">
         <v>48</v>
       </c>
@@ -2787,7 +2954,7 @@
         <v>17.55378203461964</v>
       </c>
     </row>
-    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D63">
         <v>49</v>
       </c>
@@ -2806,7 +2973,7 @@
         <v>16.921907652438357</v>
       </c>
     </row>
-    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D64">
         <v>50</v>
       </c>
@@ -2825,7 +2992,7 @@
         <v>16.32</v>
       </c>
     </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D65">
         <v>51</v>
       </c>
@@ -2844,7 +3011,7 @@
         <v>15.746303462636829</v>
       </c>
     </row>
-    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D66">
         <v>52</v>
       </c>
@@ -2863,7 +3030,7 @@
         <v>15.199184417724608</v>
       </c>
     </row>
-    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D67">
         <v>53</v>
       </c>
@@ -2882,7 +3049,7 @@
         <v>14.67712145847535</v>
       </c>
     </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D68">
         <v>54</v>
       </c>
@@ -2901,7 +3068,7 @@
         <v>14.178696502944049</v>
       </c>
     </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D69">
         <v>55</v>
       </c>
@@ -2920,7 +3087,7 @@
         <v>13.70258669908716</v>
       </c>
     </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D70">
         <v>56</v>
       </c>
@@ -2939,7 +3106,7 @@
         <v>13.247557046578201</v>
       </c>
     </row>
-    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D71">
         <v>57</v>
       </c>
@@ -2958,7 +3125,7 @@
         <v>12.812453664766219</v>
       </c>
     </row>
-    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D72">
         <v>58</v>
       </c>
@@ -2977,7 +3144,7 @@
         <v>12.396197643808534</v>
       </c>
     </row>
-    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D73">
         <v>59</v>
       </c>
@@ -2996,7 +3163,7 @@
         <v>11.997779422754368</v>
       </c>
     </row>
-    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D74">
         <v>60</v>
       </c>
@@ -3015,7 +3182,7 @@
         <v>11.616253644314872</v>
       </c>
     </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D75">
         <v>61</v>
       </c>
@@ -3034,7 +3201,7 @@
         <v>11.25073444132625</v>
       </c>
     </row>
-    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D76">
         <v>62</v>
       </c>
@@ -3053,7 +3220,7 @@
         <v>10.90039111458252</v>
       </c>
     </row>
-    <row r="77" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D77">
         <v>63</v>
       </c>
@@ -3072,7 +3239,7 @@
         <v>10.564444165856138</v>
       </c>
     </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D78">
         <v>64</v>
       </c>
@@ -3091,7 +3258,7 @@
         <v>10.242161653603828</v>
       </c>
     </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D79">
         <v>65</v>
       </c>
@@ -3110,7 +3277,7 @@
         <v>9.9328558421260205</v>
       </c>
     </row>
-    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D80">
         <v>66</v>
       </c>
@@ -3129,7 +3296,7 @@
         <v>9.6358801178615519</v>
       </c>
     </row>
-    <row r="81" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D81">
         <v>67</v>
       </c>
@@ -3148,7 +3315,7 @@
         <v>9.3506261490956941</v>
       </c>
     </row>
-    <row r="82" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D82">
         <v>68</v>
       </c>
@@ -3167,7 +3334,7 @@
         <v>9.0765212676775047</v>
       </c>
     </row>
-    <row r="83" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D83">
         <v>69</v>
       </c>
@@ -3186,7 +3353,7 @@
         <v>8.8130260534132301</v>
       </c>
     </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D84">
         <v>70</v>
       </c>
@@ -3205,7 +3372,7 @@
         <v>8.5596321036554688</v>
       </c>
     </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D85">
         <v>71</v>
       </c>
@@ -3224,7 +3391,7 @@
         <v>8.3158599722667716</v>
       </c>
     </row>
-    <row r="86" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D86">
         <v>72</v>
       </c>
@@ -3243,7 +3410,7 @@
         <v>8.081257263624174</v>
       </c>
     </row>
-    <row r="87" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D87">
         <v>73</v>
       </c>
@@ -3262,7 +3429,7 @@
         <v>7.8553968686662969</v>
       </c>
     </row>
-    <row r="88" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D88">
         <v>74</v>
       </c>
@@ -3281,7 +3448,7 @@
         <v>7.6378753311842678</v>
       </c>
     </row>
-    <row r="89" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D89">
         <v>75</v>
       </c>
@@ -3300,7 +3467,7 @@
         <v>7.4283113336367776</v>
       </c>
     </row>
-    <row r="90" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D90">
         <v>76</v>
       </c>
@@ -3319,7 +3486,7 @@
         <v>7.226344292740964</v>
       </c>
     </row>
-    <row r="91" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D91">
         <v>77</v>
       </c>
@@ -3338,7 +3505,7 @@
         <v>7.0316330559661999</v>
       </c>
     </row>
-    <row r="92" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D92">
         <v>78</v>
       </c>
@@ -3357,7 +3524,7 @@
         <v>6.8438546908477855</v>
       </c>
     </row>
-    <row r="93" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D93">
         <v>79</v>
       </c>
@@ -3376,7 +3543,7 @@
         <v>6.6627033597504717</v>
       </c>
     </row>
-    <row r="94" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D94">
         <v>80</v>
       </c>
@@ -3395,7 +3562,7 @@
         <v>6.4878892733563998</v>
       </c>
     </row>
-    <row r="95" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D95">
         <v>81</v>
       </c>
@@ -3414,7 +3581,7 @@
         <v>6.3191377167349616</v>
       </c>
     </row>
-    <row r="96" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D96">
         <v>82</v>
       </c>
@@ -3433,7 +3600,7 @@
         <v>6.1561881423801257</v>
       </c>
     </row>
-    <row r="97" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D97">
         <v>83</v>
       </c>
@@ -3452,7 +3619,7 @@
         <v>5.9987933250791521</v>
       </c>
     </row>
-    <row r="98" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D98">
         <v>84</v>
       </c>
@@ -3471,7 +3638,7 @@
         <v>5.8467185739105938</v>
       </c>
     </row>
-    <row r="99" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D99">
         <v>85</v>
       </c>
@@ -3490,7 +3657,7 @@
         <v>5.6997409970635164</v>
       </c>
     </row>
-    <row r="100" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D100">
         <v>86</v>
       </c>
@@ -3509,7 +3676,7 @@
         <v>5.557648815527731</v>
       </c>
     </row>
-    <row r="101" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D101">
         <v>87</v>
       </c>
@@ -3528,7 +3695,7 @@
         <v>5.4202407220304805</v>
       </c>
     </row>
-    <row r="102" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D102">
         <v>88</v>
       </c>
@@ -3547,7 +3714,7 @@
         <v>5.2873252818911549</v>
       </c>
     </row>
-    <row r="103" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D103">
         <v>89</v>
       </c>
@@ -3566,7 +3733,7 @@
         <v>5.1587203727355524</v>
       </c>
     </row>
-    <row r="104" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D104">
         <v>90</v>
       </c>
@@ -3585,7 +3752,7 @@
         <v>5.0342526602570432</v>
       </c>
     </row>
-    <row r="105" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D105">
         <v>91</v>
       </c>
@@ -3604,7 +3771,7 @@
         <v>4.9137571074365249</v>
       </c>
     </row>
-    <row r="106" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D106">
         <v>92</v>
       </c>
@@ -3623,7 +3790,7 @@
         <v>4.7970765148377517</v>
       </c>
     </row>
-    <row r="107" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D107">
         <v>93</v>
       </c>
@@ -3642,7 +3809,7 @@
         <v>4.6840610897818973</v>
       </c>
     </row>
-    <row r="108" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D108">
         <v>94</v>
       </c>
@@ -3661,7 +3828,7 @@
         <v>4.5745680423762147</v>
       </c>
     </row>
-    <row r="109" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D109">
         <v>95</v>
       </c>
@@ -3680,7 +3847,7 @@
         <v>4.4684612065283353</v>
       </c>
     </row>
-    <row r="110" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D110">
         <v>96</v>
       </c>
@@ -3699,7 +3866,7 @@
         <v>4.3656106842209645</v>
       </c>
     </row>
-    <row r="111" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D111">
         <v>97</v>
       </c>
@@ -3718,7 +3885,7 @@
         <v>4.2658925114532096</v>
       </c>
     </row>
-    <row r="112" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D112">
         <v>98</v>
       </c>
@@ -3737,7 +3904,7 @@
         <v>4.1691883443750886</v>
       </c>
     </row>
-    <row r="113" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D113">
         <v>99</v>
       </c>
@@ -3756,7 +3923,7 @@
         <v>4.0753851642523271</v>
       </c>
     </row>
-    <row r="114" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D114">
         <v>100</v>
       </c>
@@ -3775,7 +3942,7 @@
         <v>3.984375</v>
       </c>
     </row>
-    <row r="115" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D115">
         <v>101</v>
       </c>
@@ -3794,7 +3961,7 @@
         <v>3.8960546671167338</v>
       </c>
     </row>
-    <row r="116" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D116">
         <v>102</v>
       </c>
@@ -3813,7 +3980,7 @@
         <v>3.8103255219368948</v>
       </c>
     </row>
-    <row r="117" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D117">
         <v>103</v>
       </c>
@@ -3832,7 +3999,7 @@
         <v>3.7270932301970152</v>
       </c>
     </row>
-    <row r="118" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D118">
         <v>104</v>
       </c>
@@ -3851,7 +4018,7 @@
         <v>3.6462675489852452</v>
       </c>
     </row>
-    <row r="119" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D119">
         <v>105</v>
       </c>
@@ -3870,7 +4037,7 @@
         <v>3.5677621212094706</v>
       </c>
     </row>
-    <row r="120" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D120">
         <v>106</v>
       </c>
@@ -3889,7 +4056,7 @@
         <v>3.4914942817812791</v>
       </c>
     </row>
-    <row r="121" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D121">
         <v>107</v>
       </c>
@@ -3908,7 +4075,7 @@
         <v>3.4173848747697977</v>
       </c>
     </row>
-    <row r="122" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D122">
         <v>108</v>
       </c>
@@ -3927,7 +4094,7 @@
         <v>3.3453580808318266</v>
       </c>
     </row>
-    <row r="123" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D123">
         <v>109</v>
       </c>
@@ -3946,7 +4113,7 @@
         <v>3.2753412542730507</v>
       </c>
     </row>
-    <row r="124" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D124">
         <v>110</v>
       </c>
@@ -3965,7 +4132,7 @@
         <v>3.2072647691398228</v>
       </c>
     </row>
-    <row r="125" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D125">
         <v>111</v>
       </c>
@@ -3984,7 +4151,7 @@
         <v>3.1410618737823532</v>
       </c>
     </row>
-    <row r="126" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D126">
         <v>112</v>
       </c>
@@ -4003,7 +4170,7 @@
         <v>3.0766685533683025</v>
       </c>
     </row>
-    <row r="127" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D127">
         <v>113</v>
       </c>
@@ -4022,7 +4189,7 @@
         <v>3.0140233998611832</v>
       </c>
     </row>
-    <row r="128" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D128">
         <v>114</v>
       </c>
@@ -4041,7 +4208,7 @@
         <v>2.9530674890106514</v>
       </c>
     </row>
-    <row r="129" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D129">
         <v>115</v>
       </c>
@@ -4060,7 +4227,7 @@
         <v>2.8937442639321742</v>
       </c>
     </row>
-    <row r="130" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D130">
         <v>116</v>
       </c>
@@ -4079,7 +4246,7 @@
         <v>2.8359994248815608</v>
       </c>
     </row>
-    <row r="131" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D131">
         <v>117</v>
       </c>
@@ -4098,7 +4265,7 @@
         <v>2.7797808248560285</v>
       </c>
     </row>
-    <row r="132" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D132">
         <v>118</v>
       </c>
@@ -4117,7 +4284,7 @@
         <v>2.7250383706775443</v>
       </c>
     </row>
-    <row r="133" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D133">
         <v>119</v>
       </c>
@@ -4136,7 +4303,7 @@
         <v>2.6717239292366983</v>
       </c>
     </row>
-    <row r="134" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D134">
         <v>120</v>
       </c>
@@ -4155,7 +4322,7 @@
         <v>2.6197912385962034</v>
       </c>
     </row>
-    <row r="135" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D135">
         <v>121</v>
       </c>
@@ -4174,7 +4341,7 @@
         <v>2.5691958236724437</v>
       </c>
     </row>
-    <row r="136" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D136">
         <v>122</v>
       </c>
@@ -4193,7 +4360,7 @@
         <v>2.5198949162315776</v>
       </c>
     </row>
-    <row r="137" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D137">
         <v>123</v>
       </c>
@@ -4212,7 +4379,7 @@
         <v>2.4718473789533681</v>
       </c>
     </row>
-    <row r="138" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D138">
         <v>124</v>
       </c>
@@ -4231,7 +4398,7 @@
         <v>2.425013633331548</v>
       </c>
     </row>
-    <row r="139" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D139">
         <v>125</v>
       </c>
@@ -4250,7 +4417,7 @@
         <v>2.3793555911940514</v>
       </c>
     </row>
-    <row r="140" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D140">
         <v>126</v>
       </c>
@@ -4269,7 +4436,7 @@
         <v>2.3348365896398886</v>
       </c>
     </row>
-    <row r="141" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D141">
         <v>127</v>
       </c>
@@ -4288,7 +4455,7 @@
         <v>2.2914213292021128</v>
       </c>
     </row>
-    <row r="142" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D142">
         <v>128</v>
       </c>
@@ -4307,7 +4474,7 @@
         <v>2.2490758150580197</v>
       </c>
     </row>
-    <row r="143" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D143">
         <v>129</v>
       </c>
@@ -4326,7 +4493,7 @@
         <v>2.2077673011186718</v>
       </c>
     </row>
-    <row r="144" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D144">
         <v>130</v>
       </c>
@@ -4345,7 +4512,7 @@
         <v>2.1674642368400914</v>
       </c>
     </row>
-    <row r="145" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D145">
         <v>131</v>
       </c>
@@ -4364,7 +4531,7 @@
         <v>2.1281362166079472</v>
       </c>
     </row>
-    <row r="146" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D146">
         <v>132</v>
       </c>
@@ -4383,7 +4550,7 @@
         <v>2.0897539315565101</v>
       </c>
     </row>
-    <row r="147" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D147">
         <v>133</v>
       </c>
@@ -4402,7 +4569,7 @@
         <v>2.0522891236909744</v>
       </c>
     </row>
-    <row r="148" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D148">
         <v>134</v>
       </c>
@@ -4421,7 +4588,7 @@
         <v>2.015714542189964</v>
       </c>
     </row>
-    <row r="149" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D149">
         <v>135</v>
       </c>
@@ -4440,97 +4607,97 @@
         <v>1.980003901772394</v>
       </c>
     </row>
-    <row r="150" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E150" s="6"/>
     </row>
-    <row r="151" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E151" s="6"/>
     </row>
-    <row r="152" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E152" s="6"/>
     </row>
-    <row r="153" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E153" s="6"/>
     </row>
-    <row r="154" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E154" s="6"/>
     </row>
-    <row r="155" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E155" s="6"/>
     </row>
-    <row r="156" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E156" s="6"/>
     </row>
-    <row r="157" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E157" s="6"/>
     </row>
-    <row r="158" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E158" s="6"/>
     </row>
-    <row r="159" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E159" s="6"/>
     </row>
-    <row r="160" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E160" s="6"/>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E161" s="6"/>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E162" s="6"/>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E163" s="6"/>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E164" s="6"/>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E165" s="6"/>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E166" s="6"/>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E167" s="6"/>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E168" s="6"/>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E169" s="6"/>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E170" s="6"/>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E171" s="6"/>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E172" s="6"/>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E173" s="6"/>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E174" s="6"/>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E175" s="6"/>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E176" s="6"/>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E177" s="6"/>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E178" s="6"/>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E179" s="6"/>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E180" s="6"/>
     </row>
   </sheetData>
@@ -4539,23 +4706,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F94E3F-4D34-4266-AA2E-47BA9E73B523}">
   <dimension ref="C5:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>134</v>
       </c>
@@ -4569,7 +4736,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>53</v>
       </c>
@@ -4586,7 +4753,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>53</v>
       </c>
@@ -4603,7 +4770,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>53</v>
       </c>
@@ -4623,7 +4790,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>53</v>
       </c>
@@ -4643,7 +4810,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>53</v>
       </c>
@@ -4657,7 +4824,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>53</v>
       </c>
@@ -4671,7 +4838,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>53</v>
       </c>
@@ -4685,7 +4852,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>53</v>
       </c>
@@ -4699,7 +4866,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>53</v>
       </c>
@@ -4716,7 +4883,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>53</v>
       </c>
@@ -4730,7 +4897,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>53</v>
       </c>
@@ -4744,7 +4911,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>53</v>
       </c>
@@ -4758,7 +4925,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>53</v>
       </c>
@@ -4772,7 +4939,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>53</v>
       </c>
@@ -4787,7 +4954,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>53</v>
       </c>
@@ -4801,7 +4968,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
         <v>53</v>
       </c>
@@ -4815,7 +4982,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>53</v>
       </c>
@@ -4832,7 +4999,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
         <v>53</v>
       </c>
@@ -4849,7 +5016,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="D30" t="s">
         <v>85</v>
       </c>
@@ -4857,7 +5024,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
         <v>53</v>
       </c>
@@ -4868,7 +5035,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
         <v>53</v>
       </c>
@@ -4877,7 +5044,7 @@
       </c>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
         <v>53</v>
       </c>
@@ -4888,7 +5055,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>53</v>
       </c>
@@ -4902,7 +5069,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>53</v>
       </c>
@@ -4919,7 +5086,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
         <v>53</v>
       </c>
@@ -4936,7 +5103,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>53</v>
       </c>
@@ -4953,7 +5120,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
         <v>53</v>
       </c>
@@ -4970,7 +5137,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
         <v>53</v>
       </c>
@@ -4987,7 +5154,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
         <v>53</v>
       </c>
@@ -5004,7 +5171,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
         <v>53</v>
       </c>
@@ -5015,7 +5182,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
         <v>53</v>
       </c>
@@ -5026,7 +5193,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
         <v>53</v>
       </c>
@@ -5040,7 +5207,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
         <v>53</v>
       </c>
@@ -5054,7 +5221,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
         <v>53</v>
       </c>
@@ -5077,7 +5244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D7:N35"/>
   <sheetViews>
@@ -5085,16 +5252,16 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>3</v>
       </c>
@@ -5102,7 +5269,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -5110,13 +5277,13 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E9">
         <f>SUM(E7:E8)</f>
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>0</v>
       </c>
@@ -5124,7 +5291,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>1</v>
       </c>
@@ -5132,24 +5299,24 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E15">
         <f>SUM(E13:E14)</f>
         <v>1.2999999999999998</v>
       </c>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D17">
         <v>1.2</v>
       </c>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D20">
         <f>0.6-0.35</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D21">
         <f>D20/2</f>
         <v>0.125</v>
@@ -5170,7 +5337,7 @@
         <v>168000000</v>
       </c>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D22">
         <f>D21+0.35</f>
         <v>0.47499999999999998</v>
@@ -5192,7 +5359,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.35">
       <c r="L23" s="3">
         <f>N21/I22</f>
         <v>50.4</v>
@@ -5205,7 +5372,7 @@
         <v>3360000</v>
       </c>
     </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.35">
       <c r="H24" t="s">
         <v>8</v>
       </c>
@@ -5220,7 +5387,7 @@
         <v>2.976190476190476E-7</v>
       </c>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.35">
       <c r="H25" t="s">
         <v>10</v>
       </c>
@@ -5229,7 +5396,7 @@
         <v>7.1999999999999997E-6</v>
       </c>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.35">
       <c r="H26" t="s">
         <v>11</v>
       </c>
@@ -5237,7 +5404,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.35">
       <c r="H27" t="s">
         <v>9</v>
       </c>
@@ -5246,7 +5413,7 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.35">
       <c r="H28" t="s">
         <v>12</v>
       </c>
@@ -5258,7 +5425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:14" x14ac:dyDescent="0.35">
       <c r="H30" t="s">
         <v>14</v>
       </c>
@@ -5267,7 +5434,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:14" x14ac:dyDescent="0.35">
       <c r="H31" t="s">
         <v>15</v>
       </c>
@@ -5276,7 +5443,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.35">
       <c r="H32" t="s">
         <v>17</v>
       </c>
@@ -5285,7 +5452,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H33" t="s">
         <v>18</v>
       </c>
@@ -5294,7 +5461,7 @@
         <v>5050</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H34" t="s">
         <v>16</v>
       </c>
@@ -5302,7 +5469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H35" t="s">
         <v>19</v>
       </c>
@@ -5317,7 +5484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FE3DEB-1503-471F-AAD5-9A844AF9773A}">
   <dimension ref="B4:C34"/>
   <sheetViews>
@@ -5325,23 +5492,23 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -5349,7 +5516,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -5357,7 +5524,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>32</v>
       </c>
@@ -5366,7 +5533,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>33</v>
       </c>
@@ -5374,7 +5541,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -5383,7 +5550,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>35</v>
       </c>
@@ -5392,7 +5559,7 @@
         <v>0.1087646484375</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>36</v>
       </c>
@@ -5400,7 +5567,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>37</v>
       </c>
@@ -5408,12 +5575,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -5422,7 +5589,7 @@
         <v>0.135955810546875</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>40</v>
       </c>
@@ -5430,7 +5597,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -5438,7 +5605,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>43</v>
       </c>
@@ -5446,12 +5613,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>42</v>
       </c>
@@ -5460,12 +5627,12 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>45</v>
       </c>
@@ -5479,7 +5646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0714417D-B69A-4E2E-80E2-B702A8231408}">
   <dimension ref="C3:D12"/>
   <sheetViews>
@@ -5487,9 +5654,9 @@
       <selection activeCell="T9" sqref="S9:T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C3">
         <v>11</v>
       </c>
@@ -5497,7 +5664,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C4">
         <v>11</v>
       </c>
@@ -5505,7 +5672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C5">
         <v>11</v>
       </c>
@@ -5513,7 +5680,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6">
         <v>11</v>
       </c>
@@ -5521,7 +5688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C7">
         <v>8</v>
       </c>
@@ -5529,7 +5696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C8">
         <v>8</v>
       </c>
@@ -5537,7 +5704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C9">
         <v>2</v>
       </c>
@@ -5545,7 +5712,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C10">
         <v>2</v>
       </c>
@@ -5553,7 +5720,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C12">
         <f>SUM(C3:C10)</f>
         <v>64</v>

</xml_diff>